<commit_message>
Updating Directory and Donors list
</commit_message>
<xml_diff>
--- a/SourceFiles/Ashram-Donors.xlsx
+++ b/SourceFiles/Ashram-Donors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="50" windowWidth="19420" windowHeight="8130"/>
+    <workbookView xWindow="240" yWindow="48" windowWidth="19416" windowHeight="8136"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$194</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$200</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="357">
   <si>
     <t>NAME</t>
   </si>
@@ -825,9 +825,6 @@
     <t>Malikipuram (E.G. Dist)</t>
   </si>
   <si>
-    <t>10000</t>
-  </si>
-  <si>
     <t>Kanakam (on the occation of his son's thread cermony)</t>
   </si>
   <si>
@@ -1002,9 +999,6 @@
     <t>LeelaKrishna</t>
   </si>
   <si>
-    <t>7000</t>
-  </si>
-  <si>
     <t>1,001</t>
   </si>
   <si>
@@ -1060,6 +1054,42 @@
   </si>
   <si>
     <t>Lakshmi Narasimha Charyulu</t>
+  </si>
+  <si>
+    <t>Sobhanadri Lakshmi Narasimha Charyulu</t>
+  </si>
+  <si>
+    <t>Venkata Ramana</t>
+  </si>
+  <si>
+    <t>Peda SeshaCharyulu</t>
+  </si>
+  <si>
+    <t>Jagannadapuram</t>
+  </si>
+  <si>
+    <t>Giri Prasad</t>
+  </si>
+  <si>
+    <t>Gopala Charyulu and son inlaws</t>
+  </si>
+  <si>
+    <t>JamaiOsmania</t>
+  </si>
+  <si>
+    <t>Gudipudi</t>
+  </si>
+  <si>
+    <t>Seetharamacharyulu</t>
+  </si>
+  <si>
+    <t>6,000</t>
+  </si>
+  <si>
+    <t>7,000</t>
+  </si>
+  <si>
+    <t>7,722</t>
   </si>
 </sst>
 </file>
@@ -1542,20 +1572,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F194"/>
+  <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="D191" sqref="D191"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C197" sqref="C197"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.26953125" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.6328125" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="7.77734375" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.6640625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -1563,16 +1593,16 @@
         <v>114</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>314</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>315</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>1</v>
@@ -1603,7 +1633,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>134</v>
@@ -1623,7 +1653,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>134</v>
@@ -1643,7 +1673,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>134</v>
@@ -1663,7 +1693,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>137</v>
@@ -1683,7 +1713,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>134</v>
@@ -1703,7 +1733,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>138</v>
@@ -1723,7 +1753,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="12" t="s">
@@ -1741,7 +1771,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>132</v>
@@ -1781,7 +1811,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>140</v>
@@ -1821,7 +1851,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>132</v>
@@ -1841,7 +1871,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>137</v>
@@ -1861,7 +1891,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>142</v>
@@ -1881,7 +1911,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>132</v>
@@ -1901,7 +1931,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>140</v>
@@ -1921,7 +1951,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>141</v>
@@ -1941,7 +1971,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>132</v>
@@ -1961,7 +1991,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>134</v>
@@ -1981,13 +2011,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>139</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>113</v>
@@ -2021,13 +2051,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>140</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>17</v>
@@ -2041,7 +2071,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>143</v>
@@ -2061,7 +2091,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C26" s="21" t="s">
         <v>140</v>
@@ -2087,7 +2117,7 @@
         <v>137</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>21</v>
@@ -2101,7 +2131,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>134</v>
@@ -2141,7 +2171,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C30" s="21" t="s">
         <v>144</v>
@@ -2161,13 +2191,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C31" s="21" t="s">
         <v>151</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>23</v>
@@ -2181,7 +2211,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>137</v>
@@ -2201,7 +2231,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C33" s="21" t="s">
         <v>137</v>
@@ -2221,13 +2251,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C34" s="21" t="s">
         <v>139</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>67</v>
@@ -2241,19 +2271,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>274</v>
+        <v>350</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>16</v>
+        <v>351</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -2261,19 +2291,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -2281,19 +2311,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>202</v>
+        <v>274</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -2301,11 +2331,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C38" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>138</v>
+      </c>
       <c r="D38" s="12" t="s">
-        <v>79</v>
+        <v>202</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>20</v>
@@ -2319,16 +2351,14 @@
         <v>38</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>142</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C39" s="21"/>
       <c r="D39" s="12" t="s">
-        <v>208</v>
+        <v>79</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>124</v>
@@ -2339,16 +2369,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>241</v>
+        <v>208</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>124</v>
@@ -2359,16 +2389,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>150</v>
+        <v>327</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>132</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>270</v>
+        <v>241</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>124</v>
@@ -2379,251 +2409,251 @@
         <v>41</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>145</v>
+        <v>327</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>150</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="26">
         <v>42</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="18.45" x14ac:dyDescent="0.35">
       <c r="A44" s="26">
         <v>43</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C44" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="D44" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D44" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A45" s="26">
         <v>44</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A46" s="26">
         <v>45</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A47" s="26">
         <v>46</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>258</v>
+        <v>174</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A48" s="26">
         <v>47</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>197</v>
+        <v>258</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A49" s="26">
         <v>48</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>276</v>
+        <v>197</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A50" s="26">
         <v>49</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>185</v>
+        <v>275</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A51" s="26">
         <v>50</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C51" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>134</v>
+      </c>
       <c r="D51" s="12" t="s">
-        <v>80</v>
+        <v>185</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A52" s="26">
         <v>51</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>147</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C52" s="21"/>
       <c r="D52" s="12" t="s">
-        <v>259</v>
+        <v>80</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A53" s="26">
         <v>52</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C53" s="24" t="s">
-        <v>152</v>
+        <v>327</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>147</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>317</v>
+        <v>259</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A54" s="26">
         <v>53</v>
       </c>
-      <c r="B54" s="24" t="s">
-        <v>242</v>
+      <c r="B54" s="21" t="s">
+        <v>327</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E54" s="18" t="s">
         <v>39</v>
@@ -2632,38 +2662,38 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A55" s="26">
         <v>54</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>329</v>
+        <v>242</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" s="4" customFormat="1" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A56" s="26">
         <v>55</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E56" s="18" t="s">
         <v>21</v>
@@ -2672,376 +2702,376 @@
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A57" s="26">
         <v>56</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>329</v>
-      </c>
-      <c r="C57" s="23" t="s">
-        <v>325</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>326</v>
-      </c>
-      <c r="E57" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="F57" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A58" s="26">
         <v>57</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>329</v>
-      </c>
-      <c r="C58" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="E58" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+        <v>327</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>324</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="E58" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A59" s="26">
         <v>58</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C59" s="21" t="s">
         <v>132</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>340</v>
+        <v>276</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.45">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A60" s="26">
         <v>59</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>205</v>
+        <v>338</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="37" x14ac:dyDescent="0.45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="2" customFormat="1" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A61" s="26">
         <v>60</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="D61" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>111</v>
+        <v>148</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" ht="37.049999999999997" x14ac:dyDescent="0.45">
       <c r="A62" s="26">
         <v>61</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="E62" s="18" t="s">
-        <v>5</v>
+        <v>132</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>111</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A63" s="26">
         <v>62</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>329</v>
-      </c>
-      <c r="C63" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C63" s="21" t="s">
+        <v>150</v>
+      </c>
       <c r="D63" s="12" t="s">
-        <v>83</v>
+        <v>173</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A64" s="26">
         <v>63</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>329</v>
-      </c>
-      <c r="C64" s="21" t="s">
-        <v>151</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C64" s="21"/>
       <c r="D64" s="12" t="s">
-        <v>260</v>
+        <v>83</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A65" s="26">
         <v>64</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="D65" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="E65" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F65" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="E65" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A66" s="26">
         <v>65</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E66" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F66" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F66" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A67" s="26">
         <v>66</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>278</v>
+        <v>94</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A68" s="26">
         <v>67</v>
       </c>
-      <c r="B68" s="21" t="s">
-        <v>242</v>
+      <c r="B68" s="24" t="s">
+        <v>327</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>243</v>
+        <v>277</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A69" s="26">
         <v>68</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>329</v>
+        <v>242</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>174</v>
+        <v>243</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A70" s="26">
         <v>69</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>244</v>
+        <v>174</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A71" s="26">
         <v>70</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>168</v>
+        <v>244</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A72" s="26">
         <v>71</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A73" s="26">
         <v>72</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>226</v>
+        <v>175</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A74" s="26">
         <v>73</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>242</v>
+        <v>327</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A75" s="26">
         <v>74</v>
       </c>
       <c r="B75" s="21" t="s">
-        <v>329</v>
+        <v>242</v>
       </c>
       <c r="C75" s="21" t="s">
         <v>132</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>279</v>
+        <v>245</v>
       </c>
       <c r="E75" s="18" t="s">
         <v>4</v>
@@ -3050,218 +3080,218 @@
         <v>131</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A76" s="26">
         <v>75</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A77" s="26">
         <v>76</v>
       </c>
       <c r="B77" s="21" t="s">
-        <v>242</v>
+        <v>327</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A78" s="26">
         <v>77</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>329</v>
+        <v>242</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E78" s="18" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A79" s="26">
         <v>78</v>
       </c>
       <c r="B79" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
       <c r="E79" s="18" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A80" s="26">
         <v>79</v>
       </c>
       <c r="B80" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>282</v>
+        <v>304</v>
       </c>
       <c r="E80" s="18" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A81" s="26">
         <v>80</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C81" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E81" s="18" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A82" s="26">
         <v>81</v>
       </c>
       <c r="B82" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="F82" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A83" s="26">
         <v>82</v>
       </c>
       <c r="B83" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="F83" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A84" s="26">
         <v>83</v>
       </c>
       <c r="B84" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>169</v>
+        <v>285</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F84" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A85" s="26">
         <v>84</v>
       </c>
       <c r="B85" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>287</v>
+        <v>169</v>
       </c>
       <c r="E85" s="18" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="F85" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A86" s="26">
         <v>85</v>
       </c>
       <c r="B86" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C86" s="21" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>193</v>
+        <v>286</v>
       </c>
       <c r="E86" s="18" t="s">
         <v>10</v>
@@ -3270,118 +3300,118 @@
         <v>131</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A87" s="26">
         <v>86</v>
       </c>
       <c r="B87" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C87" s="21" t="s">
         <v>140</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E87" s="18" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="F87" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A88" s="26">
         <v>87</v>
       </c>
       <c r="B88" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C88" s="21" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E88" s="18" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="F88" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A89" s="26">
         <v>88</v>
       </c>
       <c r="B89" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C89" s="21" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
       <c r="E89" s="18" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A90" s="26">
         <v>89</v>
       </c>
       <c r="B90" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C90" s="21" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="E90" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F90" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A91" s="26">
         <v>90</v>
       </c>
       <c r="B91" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C91" s="21" t="s">
-        <v>288</v>
+        <v>143</v>
       </c>
       <c r="D91" s="12" t="s">
-        <v>289</v>
+        <v>209</v>
       </c>
       <c r="E91" s="18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F91" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A92" s="26">
         <v>91</v>
       </c>
       <c r="B92" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C92" s="21" t="s">
-        <v>146</v>
+        <v>287</v>
       </c>
       <c r="D92" s="12" t="s">
-        <v>199</v>
+        <v>288</v>
       </c>
       <c r="E92" s="18" t="s">
         <v>36</v>
@@ -3390,139 +3420,139 @@
         <v>131</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A93" s="26">
         <v>92</v>
       </c>
       <c r="B93" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C93" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E93" s="18" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F93" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A94" s="26">
         <v>93</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C94" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C94" s="21" t="s">
+        <v>148</v>
+      </c>
       <c r="D94" s="12" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="E94" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A95" s="26">
         <v>94</v>
       </c>
       <c r="B95" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C95" s="21" t="s">
-        <v>147</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C95" s="21"/>
       <c r="D95" s="12" t="s">
-        <v>290</v>
+        <v>228</v>
       </c>
       <c r="E95" s="18" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="F95" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A96" s="26">
         <v>95</v>
       </c>
       <c r="B96" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C96" s="21" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E96" s="18" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="F96" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A97" s="26">
         <v>96</v>
       </c>
       <c r="B97" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C97" s="21" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>170</v>
+        <v>295</v>
       </c>
       <c r="E97" s="18" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A98" s="26">
         <v>97</v>
       </c>
       <c r="B98" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>246</v>
+        <v>170</v>
       </c>
       <c r="E98" s="18" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F98" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A99" s="26">
         <v>98</v>
       </c>
       <c r="B99" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>291</v>
+        <v>246</v>
       </c>
       <c r="E99" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F99" s="7" t="s">
         <v>131</v>
@@ -3533,13 +3563,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C100" s="21" t="s">
         <v>134</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>193</v>
+        <v>290</v>
       </c>
       <c r="E100" s="18" t="s">
         <v>26</v>
@@ -3553,13 +3583,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C101" s="21" t="s">
         <v>134</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>292</v>
+        <v>193</v>
       </c>
       <c r="E101" s="18" t="s">
         <v>26</v>
@@ -3568,1768 +3598,1886 @@
         <v>131</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="26">
         <v>101</v>
       </c>
       <c r="B102" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>229</v>
+        <v>291</v>
       </c>
       <c r="E102" s="18" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="F102" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A103" s="26">
         <v>102</v>
       </c>
       <c r="B103" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C103" s="21" t="s">
         <v>147</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E103" s="18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="F103" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A104" s="26">
         <v>103</v>
       </c>
       <c r="B104" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C104" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="D104" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="E104" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F104" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E104" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F104" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" ht="18.45" x14ac:dyDescent="0.35">
       <c r="A105" s="26">
         <v>104</v>
       </c>
       <c r="B105" s="21" t="s">
-        <v>242</v>
+        <v>327</v>
       </c>
       <c r="C105" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="D105" s="17" t="s">
-        <v>269</v>
+        <v>139</v>
+      </c>
+      <c r="D105" s="15" t="s">
+        <v>247</v>
       </c>
       <c r="E105" s="17" t="s">
-        <v>267</v>
+        <v>67</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="18.45" x14ac:dyDescent="0.35">
       <c r="A106" s="26">
         <v>105</v>
       </c>
       <c r="B106" s="21" t="s">
-        <v>329</v>
+        <v>242</v>
       </c>
       <c r="C106" s="21" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="D106" s="17" t="s">
-        <v>330</v>
+        <v>268</v>
       </c>
       <c r="E106" s="17" t="s">
-        <v>331</v>
+        <v>267</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="18.45" x14ac:dyDescent="0.35">
       <c r="A107" s="26">
         <v>106</v>
       </c>
       <c r="B107" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="C107" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D107" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="E107" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="C107" s="21"/>
-      <c r="D107" s="17" t="s">
-        <v>334</v>
-      </c>
-      <c r="E107" s="17"/>
       <c r="F107" s="8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="18.45" x14ac:dyDescent="0.35">
       <c r="A108" s="26">
         <v>107</v>
       </c>
       <c r="B108" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C108" s="21" t="s">
-        <v>148</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C108" s="21"/>
       <c r="D108" s="17" t="s">
-        <v>335</v>
-      </c>
-      <c r="E108" s="17" t="s">
-        <v>35</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="E108" s="17"/>
       <c r="F108" s="8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="18.45" x14ac:dyDescent="0.35">
       <c r="A109" s="26">
         <v>108</v>
       </c>
       <c r="B109" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C109" s="21" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D109" s="17" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E109" s="17" t="s">
-        <v>337</v>
+        <v>35</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="18.45" x14ac:dyDescent="0.35">
       <c r="A110" s="26">
         <v>109</v>
       </c>
       <c r="B110" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C110" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="D110" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="E110" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F110" s="7">
-        <v>7722</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+        <v>142</v>
+      </c>
+      <c r="D110" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="E110" s="17" t="s">
+        <v>335</v>
+      </c>
+      <c r="F110" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="26">
         <v>110</v>
       </c>
       <c r="B111" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C111" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="D111" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="E111" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="F111" s="7">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+      <c r="D111" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="E111" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F111" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="26">
         <v>111</v>
       </c>
       <c r="B112" s="21" t="s">
-        <v>242</v>
+        <v>327</v>
       </c>
       <c r="C112" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="D112" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="E112" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F112" s="7" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+      <c r="D112" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="E112" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F112" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="26">
         <v>112</v>
       </c>
       <c r="B113" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C113" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="D113" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="E113" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F113" s="7">
-        <v>5116</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+        <v>352</v>
+      </c>
+      <c r="D113" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="E113" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F113" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A114" s="26">
         <v>113</v>
       </c>
       <c r="B114" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C114" s="21" t="s">
-        <v>147</v>
+        <v>297</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>231</v>
+        <v>298</v>
       </c>
       <c r="E114" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F114" s="7">
-        <v>5116</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A115" s="26">
         <v>114</v>
       </c>
       <c r="B115" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C115" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C115" s="21" t="s">
+        <v>145</v>
+      </c>
       <c r="D115" s="12" t="s">
-        <v>97</v>
+        <v>299</v>
       </c>
       <c r="E115" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F115" s="7">
-        <v>5116</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A116" s="26">
         <v>115</v>
       </c>
       <c r="B116" s="21" t="s">
-        <v>329</v>
+        <v>242</v>
       </c>
       <c r="C116" s="21" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>293</v>
+        <v>162</v>
       </c>
       <c r="E116" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F116" s="7">
-        <v>5116</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A117" s="26">
         <v>116</v>
       </c>
       <c r="B117" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C117" s="21" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="E117" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F117" s="7">
-        <v>5116</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+        <v>349</v>
+      </c>
+      <c r="E117" s="18"/>
+      <c r="F117" s="7" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A118" s="26">
         <v>117</v>
       </c>
       <c r="B118" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C118" s="21" t="s">
-        <v>303</v>
+        <v>146</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>302</v>
+        <v>200</v>
       </c>
       <c r="E118" s="18" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F118" s="7">
         <v>5116</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A119" s="26">
         <v>118</v>
       </c>
       <c r="B119" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C119" s="21" t="s">
-        <v>288</v>
+        <v>147</v>
       </c>
       <c r="D119" s="12" t="s">
-        <v>306</v>
+        <v>231</v>
       </c>
       <c r="E119" s="18" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F119" s="7">
         <v>5116</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A120" s="26">
         <v>119</v>
       </c>
       <c r="B120" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C120" s="21"/>
       <c r="D120" s="12" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="E120" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F120" s="7">
         <v>5116</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A121" s="26">
         <v>120</v>
       </c>
       <c r="B121" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C121" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C121" s="21" t="s">
+        <v>142</v>
+      </c>
       <c r="D121" s="12" t="s">
-        <v>109</v>
+        <v>292</v>
       </c>
       <c r="E121" s="18" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="F121" s="7">
         <v>5116</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A122" s="26">
         <v>121</v>
       </c>
       <c r="B122" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C122" s="21" t="s">
         <v>137</v>
       </c>
       <c r="D122" s="12" t="s">
-        <v>179</v>
+        <v>300</v>
       </c>
       <c r="E122" s="18" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="F122" s="7">
-        <v>5100</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+        <v>5116</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A123" s="26">
         <v>122</v>
       </c>
       <c r="B123" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C123" s="24" t="s">
-        <v>319</v>
+        <v>327</v>
+      </c>
+      <c r="C123" s="21" t="s">
+        <v>302</v>
       </c>
       <c r="D123" s="12" t="s">
-        <v>320</v>
+        <v>301</v>
       </c>
       <c r="E123" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F123" s="7" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+      <c r="F123" s="7">
+        <v>5116</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A124" s="26">
         <v>123</v>
       </c>
       <c r="B124" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C124" s="24" t="s">
-        <v>155</v>
+        <v>327</v>
+      </c>
+      <c r="C124" s="21" t="s">
+        <v>287</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="E124" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F124" s="7" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="F124" s="7">
+        <v>5116</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A125" s="26">
         <v>124</v>
       </c>
       <c r="B125" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C125" s="21"/>
       <c r="D125" s="12" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="E125" s="18" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="F125" s="7">
-        <v>5001</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+        <v>5116</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A126" s="26">
         <v>125</v>
       </c>
       <c r="B126" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C126" s="21" t="s">
-        <v>140</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C126" s="21"/>
       <c r="D126" s="12" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
       <c r="E126" s="18" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F126" s="7">
-        <v>5001</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+        <v>5116</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A127" s="26">
         <v>126</v>
       </c>
       <c r="B127" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="C127" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C127" s="21" t="s">
+        <v>137</v>
+      </c>
       <c r="D127" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="E127" s="18"/>
+        <v>179</v>
+      </c>
+      <c r="E127" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="F127" s="7">
-        <v>5001</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A128" s="26">
         <v>127</v>
       </c>
       <c r="B128" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="C128" s="22"/>
+        <v>327</v>
+      </c>
+      <c r="C128" s="24" t="s">
+        <v>318</v>
+      </c>
       <c r="D128" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E128" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F128" s="12" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+        <v>319</v>
+      </c>
+      <c r="E128" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F128" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A129" s="26">
         <v>128</v>
       </c>
       <c r="B129" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C129" s="21" t="s">
-        <v>134</v>
+        <v>327</v>
+      </c>
+      <c r="C129" s="24" t="s">
+        <v>155</v>
       </c>
       <c r="D129" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="E129" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F129" s="7">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.45">
+        <v>322</v>
+      </c>
+      <c r="E129" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F129" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A130" s="26">
         <v>129</v>
       </c>
       <c r="B130" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C130" s="21" t="s">
-        <v>144</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C130" s="21"/>
       <c r="D130" s="12" t="s">
-        <v>232</v>
+        <v>98</v>
       </c>
       <c r="E130" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F130" s="7">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+        <v>5001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A131" s="26">
         <v>130</v>
       </c>
       <c r="B131" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C131" s="21" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="E131" s="18" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F131" s="7">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+        <v>5001</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A132" s="26">
         <v>131</v>
       </c>
       <c r="B132" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C132" s="21" t="s">
-        <v>146</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="C132" s="21"/>
       <c r="D132" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="E132" s="18" t="s">
-        <v>49</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="E132" s="18"/>
       <c r="F132" s="7">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+        <v>5001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A133" s="26">
         <v>132</v>
       </c>
       <c r="B133" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="C133" s="21" t="s">
-        <v>154</v>
-      </c>
+      <c r="C133" s="22"/>
       <c r="D133" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="E133" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F133" s="7">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+        <v>261</v>
+      </c>
+      <c r="E133" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F133" s="12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A134" s="26">
         <v>133</v>
       </c>
       <c r="B134" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C134" s="21" t="s">
         <v>134</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="E134" s="18" t="s">
-        <v>25</v>
+        <v>303</v>
+      </c>
+      <c r="E134" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="F134" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" s="2" customFormat="1" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A135" s="26">
         <v>134</v>
       </c>
       <c r="B135" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C135" s="21" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>171</v>
+        <v>232</v>
       </c>
       <c r="E135" s="18" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F135" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A136" s="26">
         <v>135</v>
       </c>
       <c r="B136" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C136" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C136" s="21" t="s">
+        <v>152</v>
+      </c>
       <c r="D136" s="12" t="s">
-        <v>99</v>
+        <v>218</v>
       </c>
       <c r="E136" s="18" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="F136" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A137" s="26">
         <v>136</v>
       </c>
       <c r="B137" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C137" s="21" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E137" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F137" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A138" s="26">
         <v>137</v>
       </c>
       <c r="B138" s="21" t="s">
-        <v>329</v>
+        <v>242</v>
       </c>
       <c r="C138" s="21" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="E138" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F138" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A139" s="26">
         <v>138</v>
       </c>
       <c r="B139" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C139" s="21"/>
-      <c r="D139" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="E139" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F139" s="6">
+        <v>327</v>
+      </c>
+      <c r="C139" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D139" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E139" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F139" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A140" s="26">
         <v>139</v>
       </c>
       <c r="B140" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C140" s="21" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>313</v>
+        <v>171</v>
       </c>
       <c r="E140" s="18" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="F140" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A141" s="26">
         <v>140</v>
       </c>
       <c r="B141" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C141" s="21" t="s">
-        <v>140</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C141" s="21"/>
       <c r="D141" s="12" t="s">
-        <v>222</v>
+        <v>99</v>
       </c>
       <c r="E141" s="18" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F141" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A142" s="26">
         <v>141</v>
       </c>
       <c r="B142" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C142" s="21" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="D142" s="12" t="s">
-        <v>202</v>
+        <v>221</v>
       </c>
       <c r="E142" s="18" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="F142" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A143" s="26">
         <v>142</v>
       </c>
       <c r="B143" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C143" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C143" s="21" t="s">
+        <v>146</v>
+      </c>
       <c r="D143" s="12" t="s">
-        <v>100</v>
+        <v>201</v>
       </c>
       <c r="E143" s="18" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F143" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" ht="18.45" x14ac:dyDescent="0.35">
       <c r="A144" s="26">
         <v>143</v>
       </c>
       <c r="B144" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C144" s="21"/>
-      <c r="D144" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="E144" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F144" s="7">
+      <c r="D144" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="E144" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F144" s="6">
         <v>5000</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A145" s="26">
         <v>144</v>
       </c>
       <c r="B145" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C145" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C145" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="D145" s="12" t="s">
-        <v>102</v>
+        <v>312</v>
       </c>
       <c r="E145" s="18" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="F145" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A146" s="26">
         <v>145</v>
       </c>
       <c r="B146" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C146" s="21" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="D146" s="12" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E146" s="18" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="F146" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A147" s="26">
         <v>146</v>
       </c>
       <c r="B147" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C147" s="21" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D147" s="12" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="E147" s="18" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="F147" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A148" s="26">
         <v>147</v>
       </c>
       <c r="B148" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C148" s="21" t="s">
-        <v>140</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C148" s="21"/>
       <c r="D148" s="12" t="s">
-        <v>196</v>
+        <v>100</v>
       </c>
       <c r="E148" s="18" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="F148" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A149" s="26">
         <v>148</v>
       </c>
       <c r="B149" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C149" s="21"/>
       <c r="D149" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E149" s="18" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="F149" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A150" s="26">
         <v>149</v>
       </c>
       <c r="B150" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C150" s="21" t="s">
-        <v>161</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C150" s="21"/>
       <c r="D150" s="12" t="s">
-        <v>312</v>
+        <v>102</v>
       </c>
       <c r="E150" s="18" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F150" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A151" s="26">
         <v>150</v>
       </c>
       <c r="B151" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C151" s="21" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="D151" s="12" t="s">
-        <v>181</v>
+        <v>217</v>
       </c>
       <c r="E151" s="18" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="F151" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A152" s="26">
         <v>151</v>
       </c>
       <c r="B152" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C152" s="21" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="D152" s="12" t="s">
-        <v>201</v>
+        <v>234</v>
       </c>
       <c r="E152" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F152" s="7" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+      <c r="F152" s="7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A153" s="26">
         <v>152</v>
       </c>
       <c r="B153" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C153" s="21" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="D153" s="12" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="E153" s="18" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="F153" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A154" s="26">
         <v>153</v>
       </c>
       <c r="B154" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C154" s="21" t="s">
-        <v>134</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C154" s="21"/>
       <c r="D154" s="12" t="s">
-        <v>193</v>
+        <v>103</v>
       </c>
       <c r="E154" s="18" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F154" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A155" s="26">
         <v>154</v>
       </c>
       <c r="B155" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C155" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C155" s="21" t="s">
+        <v>161</v>
+      </c>
       <c r="D155" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="E155" s="18"/>
+        <v>311</v>
+      </c>
+      <c r="E155" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="F155" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A156" s="26">
         <v>155</v>
       </c>
       <c r="B156" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C156" s="21" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D156" s="12" t="s">
-        <v>311</v>
+        <v>181</v>
       </c>
       <c r="E156" s="18" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F156" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A157" s="26">
         <v>156</v>
       </c>
       <c r="B157" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C157" s="21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D157" s="12" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="E157" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F157" s="7">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+      <c r="F157" s="7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A158" s="26">
         <v>157</v>
       </c>
       <c r="B158" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C158" s="21" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="D158" s="12" t="s">
-        <v>310</v>
+        <v>180</v>
       </c>
       <c r="E158" s="18" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="F158" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A159" s="26">
         <v>158</v>
       </c>
       <c r="B159" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C159" s="21" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D159" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="E159" s="12" t="s">
-        <v>20</v>
+        <v>193</v>
+      </c>
+      <c r="E159" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="F159" s="7">
         <v>5000</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A160" s="26">
         <v>159</v>
       </c>
       <c r="B160" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C160" s="21" t="s">
-        <v>137</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C160" s="21"/>
       <c r="D160" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="E160" s="12"/>
-      <c r="F160" s="7" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+        <v>182</v>
+      </c>
+      <c r="E160" s="18"/>
+      <c r="F160" s="7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A161" s="26">
         <v>160</v>
       </c>
       <c r="B161" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C161" s="21" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="D161" s="12" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E161" s="18" t="s">
-        <v>104</v>
+        <v>65</v>
       </c>
       <c r="F161" s="7">
-        <v>3001</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A162" s="26">
         <v>161</v>
       </c>
       <c r="B162" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C162" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C162" s="21" t="s">
+        <v>134</v>
+      </c>
       <c r="D162" s="12" t="s">
-        <v>90</v>
+        <v>187</v>
       </c>
       <c r="E162" s="18" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="F162" s="7">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A163" s="26">
         <v>162</v>
       </c>
       <c r="B163" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C163" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C163" s="21" t="s">
+        <v>134</v>
+      </c>
       <c r="D163" s="12" t="s">
-        <v>89</v>
+        <v>309</v>
       </c>
       <c r="E163" s="18" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F163" s="7">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A164" s="26">
         <v>163</v>
       </c>
       <c r="B164" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C164" s="21"/>
-      <c r="D164" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E164" s="18" t="s">
-        <v>55</v>
+        <v>327</v>
+      </c>
+      <c r="C164" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D164" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="E164" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="F164" s="7">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A165" s="26">
         <v>164</v>
       </c>
       <c r="B165" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C165" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="D165" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="E165" s="18" t="s">
-        <v>338</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="D165" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="E165" s="12"/>
       <c r="F165" s="7" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A166" s="26">
         <v>165</v>
       </c>
       <c r="B166" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C166" s="21" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D166" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="E166" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F166" s="7">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
+        <v>347</v>
+      </c>
+      <c r="E166" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="F166" s="7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A167" s="26">
         <v>166</v>
       </c>
       <c r="B167" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C167" s="21" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="D167" s="12" t="s">
-        <v>188</v>
+        <v>308</v>
       </c>
       <c r="E167" s="18" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="F167" s="7">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A168" s="26">
         <v>167</v>
       </c>
       <c r="B168" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C168" s="21"/>
       <c r="D168" s="12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E168" s="18" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F168" s="7">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A169" s="26">
         <v>168</v>
       </c>
       <c r="B169" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C169" s="21" t="s">
-        <v>139</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C169" s="21"/>
       <c r="D169" s="12" t="s">
-        <v>235</v>
+        <v>89</v>
       </c>
       <c r="E169" s="18" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F169" s="7">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A170" s="26">
         <v>169</v>
       </c>
       <c r="B170" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C170" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="D170" s="12" t="s">
-        <v>234</v>
+        <v>327</v>
+      </c>
+      <c r="C170" s="21"/>
+      <c r="D170" s="18" t="s">
+        <v>91</v>
       </c>
       <c r="E170" s="18" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F170" s="7">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A171" s="26">
         <v>170</v>
       </c>
       <c r="B171" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C171" s="21"/>
-      <c r="D171" s="12" t="s">
-        <v>87</v>
+        <v>327</v>
+      </c>
+      <c r="C171" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D171" s="18" t="s">
+        <v>339</v>
       </c>
       <c r="E171" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F171" s="7">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
+        <v>336</v>
+      </c>
+      <c r="F171" s="7" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A172" s="26">
         <v>171</v>
       </c>
       <c r="B172" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C172" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C172" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="D172" s="12" t="s">
-        <v>86</v>
+        <v>307</v>
       </c>
       <c r="E172" s="18" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F172" s="7">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A173" s="26">
         <v>172</v>
       </c>
       <c r="B173" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C173" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="C173" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="D173" s="19" t="s">
-        <v>307</v>
-      </c>
-      <c r="E173" s="19" t="s">
-        <v>263</v>
-      </c>
-      <c r="F173" s="19" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D173" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="E173" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F173" s="7">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A174" s="26">
         <v>173</v>
       </c>
       <c r="B174" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C174" s="21"/>
       <c r="D174" s="12" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="E174" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F174" s="7" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="F174" s="7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A175" s="26">
         <v>174</v>
       </c>
       <c r="B175" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C175" s="21" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D175" s="12" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="E175" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F175" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="F175" s="7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A176" s="26">
         <v>175</v>
       </c>
       <c r="B176" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C176" s="21" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="D176" s="12" t="s">
-        <v>187</v>
+        <v>234</v>
       </c>
       <c r="E176" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F176" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+      <c r="F176" s="7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A177" s="26">
         <v>176</v>
       </c>
       <c r="B177" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C177" s="21" t="s">
-        <v>145</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C177" s="21"/>
       <c r="D177" s="12" t="s">
-        <v>213</v>
+        <v>87</v>
       </c>
       <c r="E177" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F177" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="F177" s="7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A178" s="26">
         <v>177</v>
       </c>
       <c r="B178" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C178" s="21" t="s">
-        <v>145</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C178" s="21"/>
       <c r="D178" s="12" t="s">
-        <v>214</v>
+        <v>86</v>
       </c>
       <c r="E178" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F178" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+      <c r="F178" s="7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A179" s="26">
         <v>178</v>
       </c>
       <c r="B179" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C179" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="D179" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="E179" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F179" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
+        <v>327</v>
+      </c>
+      <c r="C179" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="D179" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="E179" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F179" s="19" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A180" s="26">
         <v>179</v>
       </c>
       <c r="B180" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C180" s="21" t="s">
-        <v>132</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C180" s="21"/>
       <c r="D180" s="12" t="s">
-        <v>215</v>
+        <v>107</v>
       </c>
       <c r="E180" s="18" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="F180" s="7" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A181" s="26">
         <v>180</v>
       </c>
       <c r="B181" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C181" s="21" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D181" s="12" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E181" s="18" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="F181" s="7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A182" s="26">
         <v>181</v>
       </c>
       <c r="B182" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C182" s="21" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="D182" s="12" t="s">
-        <v>295</v>
+        <v>187</v>
       </c>
       <c r="E182" s="18" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="F182" s="7" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A183" s="26">
         <v>182</v>
       </c>
       <c r="B183" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C183" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C183" s="21" t="s">
+        <v>145</v>
+      </c>
       <c r="D183" s="12" t="s">
-        <v>85</v>
+        <v>213</v>
       </c>
       <c r="E183" s="18" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="F183" s="7" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A184" s="26">
         <v>183</v>
       </c>
       <c r="B184" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="C184" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C184" s="21" t="s">
+        <v>145</v>
+      </c>
       <c r="D184" s="12" t="s">
-        <v>251</v>
+        <v>214</v>
       </c>
       <c r="E184" s="18" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="F184" s="7" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A185" s="26">
         <v>184</v>
       </c>
       <c r="B185" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="C185" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C185" s="21" t="s">
+        <v>150</v>
+      </c>
       <c r="D185" s="12" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
       <c r="E185" s="18" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F185" s="7" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A186" s="26">
         <v>185</v>
       </c>
       <c r="B186" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C186" s="21" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D186" s="12" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="E186" s="18" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="F186" s="7" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A187" s="26">
         <v>186</v>
       </c>
       <c r="B187" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C187" s="21"/>
+        <v>327</v>
+      </c>
+      <c r="C187" s="21" t="s">
+        <v>156</v>
+      </c>
       <c r="D187" s="12" t="s">
-        <v>106</v>
+        <v>216</v>
       </c>
       <c r="E187" s="18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F187" s="7" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A188" s="26">
         <v>187</v>
       </c>
       <c r="B188" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="C188" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="D188" s="19" t="s">
+        <v>327</v>
+      </c>
+      <c r="C188" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="D188" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="E188" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F188" s="19" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E188" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F188" s="7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A189" s="26">
         <v>188</v>
       </c>
       <c r="B189" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C189" s="21"/>
       <c r="D189" s="12" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="E189" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F189" s="7">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="F189" s="7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A190" s="26">
         <v>189</v>
       </c>
       <c r="B190" s="21" t="s">
-        <v>329</v>
+        <v>250</v>
       </c>
       <c r="C190" s="21"/>
       <c r="D190" s="12" t="s">
-        <v>84</v>
+        <v>251</v>
       </c>
       <c r="E190" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F190" s="7">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="F190" s="7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
       <c r="A191" s="26">
         <v>190</v>
       </c>
       <c r="B191" s="21" t="s">
-        <v>329</v>
+        <v>242</v>
       </c>
       <c r="C191" s="21"/>
       <c r="D191" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="E191" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="E191" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F191" s="7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
+      <c r="A192" s="26">
+        <v>191</v>
+      </c>
+      <c r="B192" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="C192" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D192" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="E192" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F192" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
+      <c r="A193" s="26">
+        <v>192</v>
+      </c>
+      <c r="B193" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="C193" s="21"/>
+      <c r="D193" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E193" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F193" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
+      <c r="A194" s="26">
+        <v>193</v>
+      </c>
+      <c r="B194" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="C194" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D194" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="E194" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F191" s="7" t="s">
+      <c r="F194" s="19" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
+      <c r="A195" s="26">
+        <v>194</v>
+      </c>
+      <c r="B195" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="C195" s="21"/>
+      <c r="D195" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E195" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F195" s="7">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
+      <c r="A196" s="26">
+        <v>195</v>
+      </c>
+      <c r="B196" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="C196" s="21"/>
+      <c r="D196" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E196" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F196" s="7">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
+      <c r="A197" s="26">
+        <v>196</v>
+      </c>
+      <c r="B197" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="C197" s="21"/>
+      <c r="D197" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="E197" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F197" s="7" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A192" s="29"/>
-      <c r="B192" s="22"/>
-      <c r="C192" s="22"/>
-      <c r="D192" s="30"/>
-      <c r="E192" s="31"/>
-      <c r="F192" s="32"/>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A193" s="29"/>
-      <c r="B193" s="22"/>
-      <c r="C193" s="22"/>
-      <c r="D193" s="30"/>
-      <c r="E193" s="31"/>
-      <c r="F193" s="32"/>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A194" s="29"/>
-      <c r="B194" s="22"/>
-      <c r="C194" s="22"/>
-      <c r="D194" s="30"/>
-      <c r="E194" s="31"/>
-      <c r="F194" s="32"/>
+    <row r="198" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
+      <c r="A198" s="29"/>
+      <c r="B198" s="22"/>
+      <c r="C198" s="22"/>
+      <c r="D198" s="30"/>
+      <c r="E198" s="31"/>
+      <c r="F198" s="32"/>
+    </row>
+    <row r="199" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
+      <c r="A199" s="29"/>
+      <c r="B199" s="22"/>
+      <c r="C199" s="22"/>
+      <c r="D199" s="30"/>
+      <c r="E199" s="31"/>
+      <c r="F199" s="32"/>
+    </row>
+    <row r="200" spans="1:6" ht="18.45" x14ac:dyDescent="0.45">
+      <c r="A200" s="29"/>
+      <c r="B200" s="22"/>
+      <c r="C200" s="22"/>
+      <c r="D200" s="30"/>
+      <c r="E200" s="31"/>
+      <c r="F200" s="32"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F194">
+  <autoFilter ref="A1:F200">
     <sortState ref="A2:F185">
       <sortCondition ref="A1:A182"/>
     </sortState>
@@ -5350,7 +5498,7 @@
       <selection activeCell="F11" sqref="F11:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <sortState ref="F11:G17">
     <sortCondition descending="1" ref="G11"/>
@@ -5365,7 +5513,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating ashramam donors list and ashramam items list
</commit_message>
<xml_diff>
--- a/SourceFiles/Ashram-Donors.xlsx
+++ b/SourceFiles/Ashram-Donors.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$H$204</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$H$203</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="342">
   <si>
     <t>NAME</t>
   </si>
@@ -645,9 +645,6 @@
     <t>Muralikrishna</t>
   </si>
   <si>
-    <t>G.SeetharamaaCharyulu</t>
-  </si>
-  <si>
     <t xml:space="preserve">Madhusudhan </t>
   </si>
   <si>
@@ -1039,6 +1036,15 @@
   </si>
   <si>
     <t>330000</t>
+  </si>
+  <si>
+    <t>Kum.</t>
+  </si>
+  <si>
+    <t>SankarNagar</t>
+  </si>
+  <si>
+    <t>20000</t>
   </si>
 </sst>
 </file>
@@ -1562,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H204"/>
+  <dimension ref="A1:H203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C201" sqref="C201"/>
+      <selection activeCell="D205" sqref="D205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1581,28 +1587,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>287</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>288</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="30" t="s">
+        <v>327</v>
+      </c>
+      <c r="H1" s="29" t="s">
         <v>328</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1610,7 +1616,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>114</v>
@@ -1632,19 +1638,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>222</v>
+        <v>339</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="F3" s="32" t="s">
         <v>338</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>339</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="23"/>
@@ -1654,7 +1660,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>116</v>
@@ -1666,7 +1672,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="24"/>
@@ -1676,7 +1682,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>116</v>
@@ -1698,7 +1704,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>116</v>
@@ -1720,7 +1726,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>119</v>
@@ -1732,7 +1738,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="24"/>
@@ -1742,7 +1748,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>116</v>
@@ -1754,7 +1760,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="24"/>
@@ -1764,19 +1770,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>120</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="24"/>
@@ -1786,7 +1792,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="7" t="s">
@@ -1806,13 +1812,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>114</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>7</v>
@@ -1828,13 +1834,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>121</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>8</v>
@@ -1850,7 +1856,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>122</v>
@@ -1872,13 +1878,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>123</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>112</v>
@@ -1894,13 +1900,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>119</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>21</v>
@@ -1909,10 +1915,10 @@
         <v>60000</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1920,13 +1926,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>114</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>93</v>
@@ -1942,7 +1948,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>119</v>
@@ -1964,13 +1970,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>126</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>13</v>
@@ -1979,10 +1985,10 @@
         <v>50011</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1990,7 +1996,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>124</v>
@@ -2012,7 +2018,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>114</v>
@@ -2034,13 +2040,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>122</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>13</v>
@@ -2056,13 +2062,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>123</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>14</v>
@@ -2078,7 +2084,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>114</v>
@@ -2100,7 +2106,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>116</v>
@@ -2122,13 +2128,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>121</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>113</v>
@@ -2144,13 +2150,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>114</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>73</v>
@@ -2166,13 +2172,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>122</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>17</v>
@@ -2188,7 +2194,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>125</v>
@@ -2210,7 +2216,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>122</v>
@@ -2232,13 +2238,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>143</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>16</v>
@@ -2247,10 +2253,10 @@
         <v>32500</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H30" s="24" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -2258,7 +2264,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>116</v>
@@ -2280,13 +2286,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>114</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>78</v>
@@ -2302,13 +2308,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>133</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>23</v>
@@ -2324,7 +2330,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>119</v>
@@ -2346,7 +2352,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>119</v>
@@ -2368,13 +2374,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>121</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>67</v>
@@ -2390,16 +2396,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>132</v>
       </c>
       <c r="D37" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="E37" s="13" t="s">
         <v>316</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>317</v>
       </c>
       <c r="F37" s="32">
         <v>25000</v>
@@ -2412,13 +2418,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>132</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>44</v>
@@ -2434,7 +2440,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C39" s="16" t="s">
         <v>120</v>
@@ -2456,7 +2462,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="7" t="s">
@@ -2476,7 +2482,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>124</v>
@@ -2498,13 +2504,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C42" s="16" t="s">
         <v>114</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>66</v>
@@ -2520,13 +2526,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>132</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>35</v>
@@ -2542,13 +2548,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>127</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E44" s="13" t="s">
         <v>36</v>
@@ -2557,10 +2563,10 @@
         <v>20000</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -2568,13 +2574,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>124</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>25</v>
@@ -2583,10 +2589,10 @@
         <v>20000</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -2594,19 +2600,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>205</v>
+        <v>252</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F46" s="32">
-        <v>16116</v>
+        <v>4</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>341</v>
       </c>
       <c r="G46" s="7"/>
       <c r="H46" s="24"/>
@@ -2616,19 +2622,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="F47" s="32">
-        <v>15000</v>
+        <v>317</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>341</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="24"/>
@@ -2638,19 +2644,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F48" s="32">
-        <v>11493</v>
+        <v>16116</v>
       </c>
       <c r="G48" s="7"/>
       <c r="H48" s="24"/>
@@ -2660,19 +2666,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>5</v>
+        <v>122</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>108</v>
       </c>
       <c r="F49" s="32">
-        <v>10116</v>
+        <v>15000</v>
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="24"/>
@@ -2682,19 +2688,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F50" s="32">
-        <v>10116</v>
+        <v>11493</v>
       </c>
       <c r="G50" s="7"/>
       <c r="H50" s="24"/>
@@ -2704,16 +2710,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>238</v>
+        <v>159</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F51" s="32">
         <v>10116</v>
@@ -2726,16 +2732,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F52" s="32">
         <v>10116</v>
@@ -2748,16 +2754,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F53" s="32">
         <v>10116</v>
@@ -2770,16 +2776,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F54" s="32">
         <v>10116</v>
@@ -2792,14 +2798,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C55" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>114</v>
+      </c>
       <c r="D55" s="7" t="s">
-        <v>80</v>
+        <v>249</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="F55" s="32">
         <v>10116</v>
@@ -2812,16 +2820,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>239</v>
+        <v>165</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="F56" s="32">
         <v>10116</v>
@@ -2834,16 +2842,14 @@
         <v>56</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C57" s="19" t="s">
-        <v>134</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C57" s="16"/>
       <c r="D57" s="7" t="s">
-        <v>290</v>
+        <v>80</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F57" s="32">
         <v>10116</v>
@@ -2855,17 +2861,17 @@
       <c r="A58" s="16">
         <v>57</v>
       </c>
-      <c r="B58" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="C58" s="19" t="s">
-        <v>114</v>
+      <c r="B58" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>129</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>291</v>
+        <v>238</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="F58" s="32">
         <v>10116</v>
@@ -2877,39 +2883,39 @@
       <c r="A59" s="16">
         <v>58</v>
       </c>
-      <c r="B59" s="19" t="s">
-        <v>299</v>
+      <c r="B59" s="16" t="s">
+        <v>298</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F59" s="32">
         <v>10116</v>
       </c>
-      <c r="G59" s="31"/>
-      <c r="H59" s="25"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="24"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="16">
         <v>59</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>299</v>
+        <v>221</v>
       </c>
       <c r="C60" s="19" t="s">
         <v>114</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F60" s="32">
         <v>10116</v>
@@ -2922,38 +2928,38 @@
         <v>60</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>297</v>
+        <v>128</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="F61" s="32">
         <v>10116</v>
       </c>
-      <c r="G61" s="7"/>
-      <c r="H61" s="24"/>
+      <c r="G61" s="31"/>
+      <c r="H61" s="25"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="16">
         <v>61</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="C62" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="C62" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D62" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="E62" s="22" t="s">
-        <v>40</v>
+      <c r="D62" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="F62" s="32">
         <v>10116</v>
@@ -2966,19 +2972,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>114</v>
+        <v>298</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>296</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>251</v>
+        <v>297</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="F63" s="32">
-        <v>10016</v>
+        <v>10116</v>
       </c>
       <c r="G63" s="7"/>
       <c r="H63" s="24"/>
@@ -2988,41 +2994,41 @@
         <v>63</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="C64" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="E64" s="13" t="s">
-        <v>82</v>
+        <v>298</v>
+      </c>
+      <c r="C64" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>40</v>
       </c>
       <c r="F64" s="32">
-        <v>10001</v>
-      </c>
-      <c r="G64" s="11"/>
-      <c r="H64" s="23"/>
-    </row>
-    <row r="65" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+        <v>10116</v>
+      </c>
+      <c r="G64" s="7"/>
+      <c r="H64" s="24"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="16">
         <v>64</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C65" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D65" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>111</v>
+      <c r="D65" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="F65" s="32">
-        <v>10001</v>
+        <v>10016</v>
       </c>
       <c r="G65" s="7"/>
       <c r="H65" s="24"/>
@@ -3032,36 +3038,38 @@
         <v>65</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>153</v>
+        <v>185</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="F66" s="32">
         <v>10001</v>
       </c>
-      <c r="G66" s="7"/>
-      <c r="H66" s="24"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G66" s="11"/>
+      <c r="H66" s="23"/>
+    </row>
+    <row r="67" spans="1:8" ht="36" x14ac:dyDescent="0.35">
       <c r="A67" s="16">
         <v>66</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="C67" s="16"/>
-      <c r="D67" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>72</v>
+        <v>298</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="F67" s="32">
         <v>10001</v>
@@ -3074,19 +3082,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>240</v>
+        <v>153</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F68" s="32">
-        <v>10000</v>
+        <v>10001</v>
       </c>
       <c r="G68" s="7"/>
       <c r="H68" s="24"/>
@@ -3096,19 +3104,17 @@
         <v>68</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="C69" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>75</v>
+        <v>298</v>
+      </c>
+      <c r="C69" s="16"/>
+      <c r="D69" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="F69" s="32">
-        <v>10000</v>
+        <v>10001</v>
       </c>
       <c r="G69" s="7"/>
       <c r="H69" s="24"/>
@@ -3118,16 +3124,16 @@
         <v>69</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>94</v>
+        <v>239</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F70" s="32">
         <v>10000</v>
@@ -3140,16 +3146,16 @@
         <v>70</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="E71" s="13" t="s">
-        <v>25</v>
+        <v>124</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="F71" s="32">
         <v>10000</v>
@@ -3161,17 +3167,17 @@
       <c r="A72" s="16">
         <v>71</v>
       </c>
-      <c r="B72" s="16" t="s">
-        <v>222</v>
+      <c r="B72" s="19" t="s">
+        <v>298</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>223</v>
+        <v>94</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F72" s="32">
         <v>10000</v>
@@ -3183,17 +3189,17 @@
       <c r="A73" s="16">
         <v>72</v>
       </c>
-      <c r="B73" s="16" t="s">
-        <v>299</v>
+      <c r="B73" s="19" t="s">
+        <v>298</v>
       </c>
       <c r="C73" s="16" t="s">
         <v>114</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>154</v>
+        <v>251</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F73" s="32">
         <v>10000</v>
@@ -3206,16 +3212,16 @@
         <v>73</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>299</v>
+        <v>221</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F74" s="32">
         <v>10000</v>
@@ -3228,16 +3234,16 @@
         <v>74</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F75" s="32">
         <v>10000</v>
@@ -3250,16 +3256,16 @@
         <v>75</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>155</v>
+        <v>223</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F76" s="32">
         <v>10000</v>
@@ -3272,16 +3278,16 @@
         <v>76</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>206</v>
+        <v>148</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F77" s="32">
         <v>10000</v>
@@ -3294,16 +3300,16 @@
         <v>77</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>222</v>
+        <v>298</v>
       </c>
       <c r="C78" s="16" t="s">
         <v>114</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>225</v>
+        <v>155</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F78" s="32">
         <v>10000</v>
@@ -3316,16 +3322,16 @@
         <v>78</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>253</v>
+        <v>206</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="F79" s="32">
         <v>10000</v>
@@ -3338,16 +3344,16 @@
         <v>79</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>299</v>
+        <v>221</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>254</v>
+        <v>224</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F80" s="32">
         <v>10000</v>
@@ -3360,16 +3366,16 @@
         <v>80</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>222</v>
+        <v>298</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F81" s="32">
         <v>10000</v>
@@ -3382,16 +3388,16 @@
         <v>81</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>299</v>
+        <v>221</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="F82" s="32">
         <v>10000</v>
@@ -3404,16 +3410,16 @@
         <v>82</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C83" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="F83" s="32">
         <v>10000</v>
@@ -3426,16 +3432,16 @@
         <v>83</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>256</v>
+        <v>277</v>
       </c>
       <c r="E84" s="13" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="F84" s="32">
         <v>10000</v>
@@ -3448,16 +3454,16 @@
         <v>84</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E85" s="13" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F85" s="32">
         <v>10000</v>
@@ -3470,16 +3476,16 @@
         <v>85</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="F86" s="32">
         <v>10000</v>
@@ -3492,16 +3498,16 @@
         <v>86</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>149</v>
+        <v>258</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="F87" s="32">
         <v>10000</v>
@@ -3514,16 +3520,16 @@
         <v>87</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C88" s="16" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>260</v>
+        <v>149</v>
       </c>
       <c r="E88" s="13" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="F88" s="32">
         <v>10000</v>
@@ -3536,13 +3542,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C89" s="16" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>173</v>
+        <v>259</v>
       </c>
       <c r="E89" s="13" t="s">
         <v>10</v>
@@ -3558,16 +3564,16 @@
         <v>89</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C90" s="16" t="s">
         <v>122</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="F90" s="32">
         <v>10000</v>
@@ -3580,16 +3586,16 @@
         <v>90</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C91" s="16" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="F91" s="32">
         <v>10000</v>
@@ -3602,16 +3608,16 @@
         <v>91</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C92" s="16" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F92" s="32">
         <v>10000</v>
@@ -3624,16 +3630,16 @@
         <v>92</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C93" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F93" s="32">
         <v>10000</v>
@@ -3646,16 +3652,16 @@
         <v>93</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C94" s="16" t="s">
-        <v>261</v>
+        <v>125</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>262</v>
+        <v>189</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F94" s="32">
         <v>10000</v>
@@ -3668,13 +3674,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C95" s="16" t="s">
-        <v>128</v>
+        <v>260</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>179</v>
+        <v>261</v>
       </c>
       <c r="E95" s="13" t="s">
         <v>36</v>
@@ -3690,16 +3696,16 @@
         <v>95</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C96" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F96" s="32">
         <v>10000</v>
@@ -3712,14 +3718,16 @@
         <v>96</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C97" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="D97" s="7" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F97" s="32">
         <v>10000</v>
@@ -3732,13 +3740,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C98" s="16" t="s">
         <v>129</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E98" s="13" t="s">
         <v>74</v>
@@ -3754,13 +3762,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C99" s="16" t="s">
         <v>133</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E99" s="13" t="s">
         <v>25</v>
@@ -3776,7 +3784,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C100" s="16" t="s">
         <v>132</v>
@@ -3793,18 +3801,18 @@
       <c r="G100" s="7"/>
       <c r="H100" s="24"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="16">
         <v>100</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C101" s="16" t="s">
         <v>127</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E101" s="13" t="s">
         <v>25</v>
@@ -3820,13 +3828,13 @@
         <v>101</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C102" s="16" t="s">
         <v>116</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E102" s="13" t="s">
         <v>26</v>
@@ -3842,7 +3850,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C103" s="16" t="s">
         <v>116</v>
@@ -3859,18 +3867,18 @@
       <c r="G103" s="12"/>
       <c r="H103" s="26"/>
     </row>
-    <row r="104" spans="1:8" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="16">
         <v>103</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C104" s="16" t="s">
         <v>116</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E104" s="13" t="s">
         <v>26</v>
@@ -3886,13 +3894,13 @@
         <v>104</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C105" s="16" t="s">
         <v>129</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E105" s="13" t="s">
         <v>64</v>
@@ -3908,13 +3916,13 @@
         <v>105</v>
       </c>
       <c r="B106" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C106" s="16" t="s">
         <v>129</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E106" s="13" t="s">
         <v>74</v>
@@ -3930,13 +3938,13 @@
         <v>106</v>
       </c>
       <c r="B107" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C107" s="16" t="s">
         <v>121</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E107" s="12" t="s">
         <v>67</v>
@@ -3952,16 +3960,16 @@
         <v>107</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C108" s="16" t="s">
         <v>136</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F108" s="32">
         <v>10000</v>
@@ -3974,16 +3982,16 @@
         <v>108</v>
       </c>
       <c r="B109" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C109" s="16" t="s">
         <v>114</v>
       </c>
       <c r="D109" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="E109" s="12" t="s">
         <v>300</v>
-      </c>
-      <c r="E109" s="12" t="s">
-        <v>301</v>
       </c>
       <c r="F109" s="32">
         <v>10000</v>
@@ -3996,11 +4004,11 @@
         <v>109</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C110" s="16"/>
       <c r="D110" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E110" s="12"/>
       <c r="F110" s="32">
@@ -4014,13 +4022,13 @@
         <v>110</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C111" s="16" t="s">
         <v>130</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E111" s="12" t="s">
         <v>35</v>
@@ -4036,16 +4044,16 @@
         <v>111</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C112" s="16" t="s">
         <v>124</v>
       </c>
       <c r="D112" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="E112" s="12" t="s">
         <v>305</v>
-      </c>
-      <c r="E112" s="12" t="s">
-        <v>306</v>
       </c>
       <c r="F112" s="32">
         <v>10000</v>
@@ -4058,13 +4066,13 @@
         <v>112</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C113" s="16" t="s">
         <v>114</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E113" s="12" t="s">
         <v>4</v>
@@ -4080,13 +4088,13 @@
         <v>113</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C114" s="16" t="s">
         <v>114</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E114" s="12" t="s">
         <v>25</v>
@@ -4102,16 +4110,16 @@
         <v>114</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C115" s="16" t="s">
-        <v>318</v>
+        <v>114</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="E115" s="12" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="F115" s="32">
         <v>10000</v>
@@ -4124,19 +4132,19 @@
         <v>115</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C116" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D116" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="E116" s="12" t="s">
-        <v>25</v>
+        <v>270</v>
+      </c>
+      <c r="D116" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E116" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="F116" s="32">
-        <v>10000</v>
+        <v>7722</v>
       </c>
       <c r="G116" s="7"/>
       <c r="H116" s="24"/>
@@ -4146,19 +4154,19 @@
         <v>116</v>
       </c>
       <c r="B117" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C117" s="16" t="s">
-        <v>271</v>
+        <v>127</v>
       </c>
       <c r="D117" s="7" t="s">
         <v>272</v>
       </c>
       <c r="E117" s="13" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="F117" s="32">
-        <v>7722</v>
+        <v>7000</v>
       </c>
       <c r="G117" s="7"/>
       <c r="H117" s="24"/>
@@ -4168,16 +4176,16 @@
         <v>117</v>
       </c>
       <c r="B118" s="16" t="s">
-        <v>299</v>
+        <v>221</v>
       </c>
       <c r="C118" s="16" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="D118" s="7" t="s">
-        <v>273</v>
+        <v>144</v>
       </c>
       <c r="E118" s="13" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="F118" s="32">
         <v>7000</v>
@@ -4190,19 +4198,17 @@
         <v>118</v>
       </c>
       <c r="B119" s="16" t="s">
-        <v>222</v>
+        <v>298</v>
       </c>
       <c r="C119" s="16" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E119" s="13" t="s">
-        <v>39</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="E119" s="13"/>
       <c r="F119" s="32">
-        <v>7000</v>
+        <v>6000</v>
       </c>
       <c r="G119" s="7"/>
       <c r="H119" s="24"/>
@@ -4212,17 +4218,19 @@
         <v>119</v>
       </c>
       <c r="B120" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C120" s="16" t="s">
         <v>128</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="E120" s="13"/>
+        <v>180</v>
+      </c>
+      <c r="E120" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="F120" s="32">
-        <v>6000</v>
+        <v>5116</v>
       </c>
       <c r="G120" s="7"/>
       <c r="H120" s="24"/>
@@ -4232,16 +4240,16 @@
         <v>120</v>
       </c>
       <c r="B121" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C121" s="16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="E121" s="13" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F121" s="32">
         <v>5116</v>
@@ -4254,16 +4262,14 @@
         <v>121</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C122" s="16" t="s">
-        <v>129</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C122" s="16"/>
       <c r="D122" s="7" t="s">
-        <v>211</v>
+        <v>97</v>
       </c>
       <c r="E122" s="13" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="F122" s="32">
         <v>5116</v>
@@ -4276,14 +4282,16 @@
         <v>122</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C123" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C123" s="16" t="s">
+        <v>124</v>
+      </c>
       <c r="D123" s="7" t="s">
-        <v>97</v>
+        <v>265</v>
       </c>
       <c r="E123" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F123" s="32">
         <v>5116</v>
@@ -4296,16 +4304,16 @@
         <v>123</v>
       </c>
       <c r="B124" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C124" s="16" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="E124" s="13" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F124" s="32">
         <v>5116</v>
@@ -4318,16 +4326,16 @@
         <v>124</v>
       </c>
       <c r="B125" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C125" s="16" t="s">
-        <v>119</v>
+        <v>275</v>
       </c>
       <c r="D125" s="7" t="s">
         <v>274</v>
       </c>
       <c r="E125" s="13" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F125" s="32">
         <v>5116</v>
@@ -4340,16 +4348,16 @@
         <v>125</v>
       </c>
       <c r="B126" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="D126" s="7" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="E126" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F126" s="32">
         <v>5116</v>
@@ -4362,16 +4370,14 @@
         <v>126</v>
       </c>
       <c r="B127" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C127" s="16" t="s">
-        <v>261</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C127" s="16"/>
       <c r="D127" s="7" t="s">
-        <v>279</v>
+        <v>110</v>
       </c>
       <c r="E127" s="13" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="F127" s="32">
         <v>5116</v>
@@ -4384,14 +4390,14 @@
         <v>127</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C128" s="16"/>
       <c r="D128" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E128" s="13" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="F128" s="32">
         <v>5116</v>
@@ -4404,17 +4410,19 @@
         <v>128</v>
       </c>
       <c r="B129" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C129" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C129" s="16" t="s">
+        <v>119</v>
+      </c>
       <c r="D129" s="7" t="s">
-        <v>109</v>
+        <v>159</v>
       </c>
       <c r="E129" s="13" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="F129" s="32">
-        <v>5116</v>
+        <v>5100</v>
       </c>
       <c r="G129" s="7"/>
       <c r="H129" s="24"/>
@@ -4424,19 +4432,19 @@
         <v>129</v>
       </c>
       <c r="B130" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C130" s="16" t="s">
-        <v>119</v>
+        <v>298</v>
+      </c>
+      <c r="C130" s="19" t="s">
+        <v>291</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>159</v>
+        <v>292</v>
       </c>
       <c r="E130" s="13" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="F130" s="32">
-        <v>5100</v>
+        <v>5004</v>
       </c>
       <c r="G130" s="7"/>
       <c r="H130" s="24"/>
@@ -4446,16 +4454,16 @@
         <v>130</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>292</v>
+        <v>137</v>
       </c>
       <c r="D131" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E131" s="13" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F131" s="32">
         <v>5004</v>
@@ -4468,19 +4476,17 @@
         <v>131</v>
       </c>
       <c r="B132" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C132" s="19" t="s">
-        <v>137</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="C132" s="19"/>
       <c r="D132" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="E132" s="13" t="s">
-        <v>2</v>
+        <v>240</v>
+      </c>
+      <c r="E132" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="F132" s="32">
-        <v>5004</v>
+        <v>5001</v>
       </c>
       <c r="G132" s="7"/>
       <c r="H132" s="24"/>
@@ -4490,14 +4496,14 @@
         <v>132</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="C133" s="19"/>
+        <v>298</v>
+      </c>
+      <c r="C133" s="16"/>
       <c r="D133" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="E133" s="7" t="s">
-        <v>37</v>
+        <v>98</v>
+      </c>
+      <c r="E133" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="F133" s="32">
         <v>5001</v>
@@ -4510,14 +4516,16 @@
         <v>133</v>
       </c>
       <c r="B134" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C134" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C134" s="16" t="s">
+        <v>122</v>
+      </c>
       <c r="D134" s="7" t="s">
-        <v>98</v>
+        <v>175</v>
       </c>
       <c r="E134" s="13" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F134" s="32">
         <v>5001</v>
@@ -4530,17 +4538,13 @@
         <v>134</v>
       </c>
       <c r="B135" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C135" s="16" t="s">
-        <v>122</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="C135" s="16"/>
       <c r="D135" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E135" s="13" t="s">
-        <v>40</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="E135" s="13"/>
       <c r="F135" s="32">
         <v>5001</v>
       </c>
@@ -4552,75 +4556,79 @@
         <v>135</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="C136" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C136" s="28" t="s">
+        <v>116</v>
+      </c>
       <c r="D136" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="E136" s="13"/>
+        <v>276</v>
+      </c>
+      <c r="E136" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="F136" s="32">
-        <v>5001</v>
+        <v>5000</v>
       </c>
       <c r="G136" s="7"/>
       <c r="H136" s="24"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A137" s="16">
         <v>136</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C137" s="28" t="s">
-        <v>116</v>
+        <v>298</v>
+      </c>
+      <c r="C137" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="D137" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="E137" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E137" s="13" t="s">
         <v>26</v>
       </c>
       <c r="F137" s="32">
         <v>5000</v>
       </c>
-      <c r="G137" s="7"/>
-      <c r="H137" s="24"/>
-    </row>
-    <row r="138" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G137" s="11"/>
+      <c r="H137" s="23"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" s="16">
         <v>137</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C138" s="16" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="D138" s="7" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="E138" s="13" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="F138" s="32">
         <v>5000</v>
       </c>
-      <c r="G138" s="11"/>
-      <c r="H138" s="23"/>
+      <c r="G138" s="7"/>
+      <c r="H138" s="24"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" s="16">
         <v>138</v>
       </c>
       <c r="B139" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C139" s="16" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D139" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E139" s="13" t="s">
         <v>49</v>
@@ -4636,16 +4644,16 @@
         <v>139</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>299</v>
+        <v>221</v>
       </c>
       <c r="C140" s="16" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D140" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E140" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F140" s="32">
         <v>5000</v>
@@ -4658,16 +4666,16 @@
         <v>140</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>222</v>
+        <v>298</v>
       </c>
       <c r="C141" s="16" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="D141" s="7" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="E141" s="13" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F141" s="32">
         <v>5000</v>
@@ -4680,16 +4688,16 @@
         <v>141</v>
       </c>
       <c r="B142" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C142" s="16" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="D142" s="7" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="E142" s="13" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F142" s="32">
         <v>5000</v>
@@ -4702,16 +4710,14 @@
         <v>142</v>
       </c>
       <c r="B143" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C143" s="16" t="s">
-        <v>132</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C143" s="16"/>
       <c r="D143" s="7" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="E143" s="13" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F143" s="32">
         <v>5000</v>
@@ -4724,14 +4730,16 @@
         <v>143</v>
       </c>
       <c r="B144" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C144" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C144" s="16" t="s">
+        <v>137</v>
+      </c>
       <c r="D144" s="7" t="s">
-        <v>99</v>
+        <v>201</v>
       </c>
       <c r="E144" s="13" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="F144" s="32">
         <v>5000</v>
@@ -4744,16 +4752,16 @@
         <v>144</v>
       </c>
       <c r="B145" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C145" s="16" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D145" s="7" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="E145" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F145" s="32">
         <v>5000</v>
@@ -4766,18 +4774,16 @@
         <v>145</v>
       </c>
       <c r="B146" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C146" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="D146" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E146" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F146" s="32">
+        <v>298</v>
+      </c>
+      <c r="C146" s="16"/>
+      <c r="D146" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E146" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F146" s="33">
         <v>5000</v>
       </c>
       <c r="G146" s="7"/>
@@ -4788,16 +4794,18 @@
         <v>146</v>
       </c>
       <c r="B147" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C147" s="16"/>
-      <c r="D147" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="E147" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F147" s="33">
+        <v>298</v>
+      </c>
+      <c r="C147" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D147" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="E147" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F147" s="32">
         <v>5000</v>
       </c>
       <c r="G147" s="7"/>
@@ -4808,16 +4816,16 @@
         <v>147</v>
       </c>
       <c r="B148" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C148" s="16" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D148" s="7" t="s">
-        <v>286</v>
+        <v>202</v>
       </c>
       <c r="E148" s="13" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F148" s="32">
         <v>5000</v>
@@ -4830,16 +4838,16 @@
         <v>148</v>
       </c>
       <c r="B149" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C149" s="16" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D149" s="7" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="E149" s="13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F149" s="32">
         <v>5000</v>
@@ -4852,13 +4860,11 @@
         <v>149</v>
       </c>
       <c r="B150" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C150" s="16" t="s">
-        <v>128</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C150" s="16"/>
       <c r="D150" s="7" t="s">
-        <v>182</v>
+        <v>100</v>
       </c>
       <c r="E150" s="13" t="s">
         <v>25</v>
@@ -4874,14 +4880,14 @@
         <v>150</v>
       </c>
       <c r="B151" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C151" s="16"/>
       <c r="D151" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E151" s="13" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="F151" s="32">
         <v>5000</v>
@@ -4894,14 +4900,14 @@
         <v>151</v>
       </c>
       <c r="B152" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C152" s="16"/>
       <c r="D152" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E152" s="13" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="F152" s="32">
         <v>5000</v>
@@ -4914,14 +4920,16 @@
         <v>152</v>
       </c>
       <c r="B153" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C153" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C153" s="16" t="s">
+        <v>142</v>
+      </c>
       <c r="D153" s="7" t="s">
-        <v>102</v>
+        <v>197</v>
       </c>
       <c r="E153" s="13" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="F153" s="32">
         <v>5000</v>
@@ -4934,16 +4942,16 @@
         <v>153</v>
       </c>
       <c r="B154" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C154" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D154" s="7" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="E154" s="13" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F154" s="32">
         <v>5000</v>
@@ -4956,13 +4964,13 @@
         <v>154</v>
       </c>
       <c r="B155" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C155" s="16" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="D155" s="7" t="s">
-        <v>214</v>
+        <v>176</v>
       </c>
       <c r="E155" s="13" t="s">
         <v>55</v>
@@ -4978,16 +4986,14 @@
         <v>155</v>
       </c>
       <c r="B156" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C156" s="16" t="s">
-        <v>122</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C156" s="16"/>
       <c r="D156" s="7" t="s">
-        <v>176</v>
+        <v>103</v>
       </c>
       <c r="E156" s="13" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="F156" s="32">
         <v>5000</v>
@@ -5000,14 +5006,16 @@
         <v>156</v>
       </c>
       <c r="B157" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C157" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C157" s="16" t="s">
+        <v>143</v>
+      </c>
       <c r="D157" s="7" t="s">
-        <v>103</v>
+        <v>284</v>
       </c>
       <c r="E157" s="13" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F157" s="32">
         <v>5000</v>
@@ -5020,16 +5028,16 @@
         <v>157</v>
       </c>
       <c r="B158" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C158" s="16" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="D158" s="7" t="s">
-        <v>285</v>
+        <v>161</v>
       </c>
       <c r="E158" s="13" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="F158" s="32">
         <v>5000</v>
@@ -5042,16 +5050,16 @@
         <v>158</v>
       </c>
       <c r="B159" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C159" s="16" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D159" s="7" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="E159" s="13" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="F159" s="32">
         <v>5000</v>
@@ -5064,16 +5072,16 @@
         <v>159</v>
       </c>
       <c r="B160" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C160" s="16" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="D160" s="7" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="E160" s="13" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="F160" s="32">
         <v>5000</v>
@@ -5086,16 +5094,16 @@
         <v>160</v>
       </c>
       <c r="B161" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C161" s="16" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="D161" s="7" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="E161" s="13" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="F161" s="32">
         <v>5000</v>
@@ -5108,17 +5116,13 @@
         <v>161</v>
       </c>
       <c r="B162" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C162" s="16" t="s">
-        <v>116</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C162" s="16"/>
       <c r="D162" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="E162" s="13" t="s">
-        <v>26</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="E162" s="13"/>
       <c r="F162" s="32">
         <v>5000</v>
       </c>
@@ -5130,13 +5134,17 @@
         <v>162</v>
       </c>
       <c r="B163" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C163" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C163" s="16" t="s">
+        <v>114</v>
+      </c>
       <c r="D163" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="E163" s="13"/>
+        <v>283</v>
+      </c>
+      <c r="E163" s="13" t="s">
+        <v>65</v>
+      </c>
       <c r="F163" s="32">
         <v>5000</v>
       </c>
@@ -5148,16 +5156,16 @@
         <v>163</v>
       </c>
       <c r="B164" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C164" s="16" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D164" s="7" t="s">
-        <v>284</v>
+        <v>167</v>
       </c>
       <c r="E164" s="13" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="F164" s="32">
         <v>5000</v>
@@ -5170,13 +5178,13 @@
         <v>164</v>
       </c>
       <c r="B165" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C165" s="16" t="s">
         <v>116</v>
       </c>
       <c r="D165" s="7" t="s">
-        <v>167</v>
+        <v>282</v>
       </c>
       <c r="E165" s="13" t="s">
         <v>26</v>
@@ -5192,16 +5200,16 @@
         <v>165</v>
       </c>
       <c r="B166" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C166" s="16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D166" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="E166" s="13" t="s">
-        <v>26</v>
+        <v>192</v>
+      </c>
+      <c r="E166" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F166" s="32">
         <v>5000</v>
@@ -5214,17 +5222,15 @@
         <v>166</v>
       </c>
       <c r="B167" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C167" s="16" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D167" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="E167" s="7" t="s">
-        <v>20</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="E167" s="7"/>
       <c r="F167" s="32">
         <v>5000</v>
       </c>
@@ -5236,15 +5242,17 @@
         <v>167</v>
       </c>
       <c r="B168" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C168" s="16" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D168" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="E168" s="7"/>
+        <v>312</v>
+      </c>
+      <c r="E168" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="F168" s="32">
         <v>5000</v>
       </c>
@@ -5256,16 +5264,16 @@
         <v>168</v>
       </c>
       <c r="B169" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C169" s="16" t="s">
-        <v>122</v>
+        <v>333</v>
       </c>
       <c r="D169" s="7" t="s">
-        <v>313</v>
+        <v>334</v>
       </c>
       <c r="E169" s="7" t="s">
-        <v>314</v>
+        <v>332</v>
       </c>
       <c r="F169" s="32">
         <v>5000</v>
@@ -5278,19 +5286,19 @@
         <v>169</v>
       </c>
       <c r="B170" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C170" s="16" t="s">
-        <v>334</v>
+        <v>136</v>
       </c>
       <c r="D170" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="E170" s="7" t="s">
-        <v>333</v>
+        <v>281</v>
+      </c>
+      <c r="E170" s="13" t="s">
+        <v>104</v>
       </c>
       <c r="F170" s="32">
-        <v>5000</v>
+        <v>3001</v>
       </c>
       <c r="G170" s="7"/>
       <c r="H170" s="24"/>
@@ -5300,19 +5308,17 @@
         <v>170</v>
       </c>
       <c r="B171" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C171" s="16" t="s">
-        <v>136</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C171" s="16"/>
       <c r="D171" s="7" t="s">
-        <v>282</v>
+        <v>90</v>
       </c>
       <c r="E171" s="13" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="F171" s="32">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="G171" s="7"/>
       <c r="H171" s="24"/>
@@ -5322,14 +5328,14 @@
         <v>171</v>
       </c>
       <c r="B172" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C172" s="16"/>
       <c r="D172" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E172" s="13" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="F172" s="32">
         <v>3000</v>
@@ -5342,14 +5348,14 @@
         <v>172</v>
       </c>
       <c r="B173" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C173" s="16"/>
-      <c r="D173" s="7" t="s">
-        <v>89</v>
+      <c r="D173" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="E173" s="13" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="F173" s="32">
         <v>3000</v>
@@ -5362,14 +5368,16 @@
         <v>173</v>
       </c>
       <c r="B174" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C174" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C174" s="16" t="s">
+        <v>132</v>
+      </c>
       <c r="D174" s="13" t="s">
-        <v>91</v>
+        <v>308</v>
       </c>
       <c r="E174" s="13" t="s">
-        <v>55</v>
+        <v>306</v>
       </c>
       <c r="F174" s="32">
         <v>3000</v>
@@ -5382,19 +5390,19 @@
         <v>174</v>
       </c>
       <c r="B175" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C175" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="D175" s="13" t="s">
-        <v>309</v>
+        <v>114</v>
+      </c>
+      <c r="D175" s="7" t="s">
+        <v>280</v>
       </c>
       <c r="E175" s="13" t="s">
-        <v>307</v>
+        <v>48</v>
       </c>
       <c r="F175" s="32">
-        <v>3000</v>
+        <v>2500</v>
       </c>
       <c r="G175" s="7"/>
       <c r="H175" s="24"/>
@@ -5404,19 +5412,19 @@
         <v>175</v>
       </c>
       <c r="B176" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C176" s="16" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D176" s="7" t="s">
-        <v>281</v>
+        <v>168</v>
       </c>
       <c r="E176" s="13" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F176" s="32">
-        <v>2500</v>
+        <v>2016</v>
       </c>
       <c r="G176" s="7"/>
       <c r="H176" s="24"/>
@@ -5426,19 +5434,17 @@
         <v>176</v>
       </c>
       <c r="B177" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C177" s="16" t="s">
-        <v>122</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C177" s="16"/>
       <c r="D177" s="7" t="s">
-        <v>168</v>
+        <v>88</v>
       </c>
       <c r="E177" s="13" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="F177" s="32">
-        <v>2016</v>
+        <v>2000</v>
       </c>
       <c r="G177" s="7"/>
       <c r="H177" s="24"/>
@@ -5448,14 +5454,16 @@
         <v>177</v>
       </c>
       <c r="B178" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C178" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C178" s="16" t="s">
+        <v>121</v>
+      </c>
       <c r="D178" s="7" t="s">
-        <v>88</v>
+        <v>214</v>
       </c>
       <c r="E178" s="13" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F178" s="32">
         <v>2000</v>
@@ -5468,16 +5476,16 @@
         <v>178</v>
       </c>
       <c r="B179" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C179" s="16" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="D179" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E179" s="13" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="F179" s="32">
         <v>2000</v>
@@ -5490,16 +5498,14 @@
         <v>179</v>
       </c>
       <c r="B180" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C180" s="16" t="s">
-        <v>139</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C180" s="16"/>
       <c r="D180" s="7" t="s">
-        <v>214</v>
+        <v>87</v>
       </c>
       <c r="E180" s="13" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="F180" s="32">
         <v>2000</v>
@@ -5512,14 +5518,14 @@
         <v>180</v>
       </c>
       <c r="B181" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C181" s="16"/>
       <c r="D181" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E181" s="13" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="F181" s="32">
         <v>2000</v>
@@ -5532,14 +5538,16 @@
         <v>181</v>
       </c>
       <c r="B182" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C182" s="16"/>
-      <c r="D182" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E182" s="13" t="s">
-        <v>63</v>
+        <v>298</v>
+      </c>
+      <c r="C182" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D182" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="E182" s="14" t="s">
+        <v>241</v>
       </c>
       <c r="F182" s="32">
         <v>2000</v>
@@ -5552,19 +5560,17 @@
         <v>182</v>
       </c>
       <c r="B183" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C183" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="D183" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="E183" s="14" t="s">
-        <v>242</v>
+        <v>298</v>
+      </c>
+      <c r="C183" s="28"/>
+      <c r="D183" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E183" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="F183" s="32">
-        <v>2000</v>
+        <v>1120</v>
       </c>
       <c r="G183" s="7"/>
       <c r="H183" s="24"/>
@@ -5574,17 +5580,19 @@
         <v>183</v>
       </c>
       <c r="B184" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C184" s="28"/>
+        <v>298</v>
+      </c>
+      <c r="C184" s="16" t="s">
+        <v>125</v>
+      </c>
       <c r="D184" s="7" t="s">
-        <v>107</v>
+        <v>190</v>
       </c>
       <c r="E184" s="13" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="F184" s="32">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="G184" s="7"/>
       <c r="H184" s="24"/>
@@ -5594,16 +5602,16 @@
         <v>184</v>
       </c>
       <c r="B185" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C185" s="16" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D185" s="7" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="E185" s="13" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="F185" s="32">
         <v>1116</v>
@@ -5616,16 +5624,16 @@
         <v>185</v>
       </c>
       <c r="B186" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C186" s="16" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="D186" s="7" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="E186" s="13" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="F186" s="32">
         <v>1116</v>
@@ -5638,16 +5646,16 @@
         <v>186</v>
       </c>
       <c r="B187" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C187" s="16" t="s">
         <v>127</v>
       </c>
       <c r="D187" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E187" s="13" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="F187" s="32">
         <v>1116</v>
@@ -5660,16 +5668,16 @@
         <v>187</v>
       </c>
       <c r="B188" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C188" s="16" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D188" s="7" t="s">
-        <v>194</v>
+        <v>152</v>
       </c>
       <c r="E188" s="13" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F188" s="32">
         <v>1116</v>
@@ -5682,19 +5690,19 @@
         <v>188</v>
       </c>
       <c r="B189" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C189" s="16" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="D189" s="7" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
       <c r="E189" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F189" s="32">
-        <v>1116</v>
+        <v>1016</v>
       </c>
       <c r="G189" s="7"/>
       <c r="H189" s="24"/>
@@ -5704,19 +5712,19 @@
         <v>189</v>
       </c>
       <c r="B190" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C190" s="16" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="D190" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E190" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F190" s="32">
-        <v>1016</v>
+        <v>1011</v>
       </c>
       <c r="G190" s="7"/>
       <c r="H190" s="24"/>
@@ -5726,19 +5734,19 @@
         <v>190</v>
       </c>
       <c r="B191" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C191" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D191" s="7" t="s">
-        <v>196</v>
+        <v>267</v>
       </c>
       <c r="E191" s="13" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="F191" s="32">
-        <v>1011</v>
+        <v>1001</v>
       </c>
       <c r="G191" s="7"/>
       <c r="H191" s="24"/>
@@ -5748,16 +5756,14 @@
         <v>191</v>
       </c>
       <c r="B192" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C192" s="16" t="s">
-        <v>136</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C192" s="16"/>
       <c r="D192" s="7" t="s">
-        <v>268</v>
+        <v>85</v>
       </c>
       <c r="E192" s="13" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="F192" s="32">
         <v>1001</v>
@@ -5770,11 +5776,11 @@
         <v>192</v>
       </c>
       <c r="B193" s="16" t="s">
-        <v>299</v>
+        <v>229</v>
       </c>
       <c r="C193" s="16"/>
       <c r="D193" s="7" t="s">
-        <v>85</v>
+        <v>230</v>
       </c>
       <c r="E193" s="13" t="s">
         <v>36</v>
@@ -5790,11 +5796,11 @@
         <v>193</v>
       </c>
       <c r="B194" s="16" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C194" s="16"/>
       <c r="D194" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E194" s="13" t="s">
         <v>36</v>
@@ -5810,17 +5816,19 @@
         <v>194</v>
       </c>
       <c r="B195" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="C195" s="16"/>
+        <v>298</v>
+      </c>
+      <c r="C195" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="D195" s="7" t="s">
-        <v>229</v>
+        <v>184</v>
       </c>
       <c r="E195" s="13" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="F195" s="32">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="G195" s="7"/>
       <c r="H195" s="24"/>
@@ -5830,16 +5838,14 @@
         <v>195</v>
       </c>
       <c r="B196" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C196" s="16" t="s">
-        <v>130</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C196" s="16"/>
       <c r="D196" s="7" t="s">
-        <v>184</v>
+        <v>106</v>
       </c>
       <c r="E196" s="13" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="F196" s="32">
         <v>1000</v>
@@ -5852,14 +5858,16 @@
         <v>196</v>
       </c>
       <c r="B197" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C197" s="16"/>
-      <c r="D197" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E197" s="13" t="s">
-        <v>25</v>
+        <v>298</v>
+      </c>
+      <c r="C197" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D197" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E197" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="F197" s="32">
         <v>1000</v>
@@ -5872,19 +5880,17 @@
         <v>197</v>
       </c>
       <c r="B198" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C198" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D198" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="E198" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="C198" s="28"/>
+      <c r="D198" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E198" s="13" t="s">
         <v>72</v>
       </c>
       <c r="F198" s="32">
-        <v>1000</v>
+        <v>520</v>
       </c>
       <c r="G198" s="7"/>
       <c r="H198" s="24"/>
@@ -5894,17 +5900,17 @@
         <v>198</v>
       </c>
       <c r="B199" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C199" s="28"/>
+        <v>298</v>
+      </c>
+      <c r="C199" s="16"/>
       <c r="D199" s="7" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="E199" s="13" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F199" s="32">
-        <v>520</v>
+        <v>501</v>
       </c>
       <c r="G199" s="7"/>
       <c r="H199" s="24"/>
@@ -5914,40 +5920,27 @@
         <v>199</v>
       </c>
       <c r="B200" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C200" s="16"/>
       <c r="D200" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E200" s="13" t="s">
-        <v>62</v>
+        <v>309</v>
+      </c>
+      <c r="E200" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="F200" s="32">
-        <v>501</v>
+        <v>120</v>
       </c>
       <c r="G200" s="7"/>
       <c r="H200" s="24"/>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A201" s="16">
-        <v>200</v>
-      </c>
-      <c r="B201" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="C201" s="16"/>
-      <c r="D201" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="E201" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F201" s="32">
-        <v>120</v>
-      </c>
-      <c r="G201" s="7"/>
-      <c r="H201" s="24"/>
+      <c r="B201" s="17"/>
+      <c r="C201" s="17"/>
+      <c r="D201" s="21"/>
+      <c r="E201" s="22"/>
+      <c r="F201" s="34"/>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B202" s="17"/>
@@ -5957,21 +5950,14 @@
       <c r="F202" s="34"/>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B203" s="17"/>
+      <c r="B203" s="16"/>
       <c r="C203" s="17"/>
       <c r="D203" s="21"/>
       <c r="E203" s="22"/>
       <c r="F203" s="34"/>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B204" s="16"/>
-      <c r="C204" s="17"/>
-      <c r="D204" s="21"/>
-      <c r="E204" s="22"/>
-      <c r="F204" s="34"/>
-    </row>
   </sheetData>
-  <autoFilter ref="B1:H204">
+  <autoFilter ref="B1:H203">
     <sortState ref="B2:I201">
       <sortCondition descending="1" ref="F1:F201"/>
     </sortState>

</xml_diff>

<commit_message>
Sravana poornima 2019 news updated donors list updated directory list
</commit_message>
<xml_diff>
--- a/SourceFiles/Ashram-Donors.xlsx
+++ b/SourceFiles/Ashram-Donors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="381">
   <si>
     <t>NAME</t>
   </si>
@@ -1026,25 +1026,142 @@
     <t xml:space="preserve"> V S R K Acharyulu in memory of his father Agnihotram PeddaSeshacharyulu</t>
   </si>
   <si>
-    <t>300000</t>
-  </si>
-  <si>
-    <t>100000</t>
-  </si>
-  <si>
     <t>SuryaVarchasvi d/o P Gopala Charyulu</t>
   </si>
   <si>
-    <t>330000</t>
-  </si>
-  <si>
     <t>Kum.</t>
   </si>
   <si>
     <t>SankarNagar</t>
   </si>
   <si>
-    <t>20000</t>
+    <t>₹ 3,50,000</t>
+  </si>
+  <si>
+    <t>₹ 3,30,000</t>
+  </si>
+  <si>
+    <t>₹ 3,00,000</t>
+  </si>
+  <si>
+    <t>₹ 1,50,000</t>
+  </si>
+  <si>
+    <t>₹ 1,00,116</t>
+  </si>
+  <si>
+    <t>₹ 1,00,000</t>
+  </si>
+  <si>
+    <t>₹ 60,000</t>
+  </si>
+  <si>
+    <t>₹ 50,116</t>
+  </si>
+  <si>
+    <t>₹ 50,011</t>
+  </si>
+  <si>
+    <t>₹ 50,000</t>
+  </si>
+  <si>
+    <t>₹ 32,500</t>
+  </si>
+  <si>
+    <t>₹ 25,000</t>
+  </si>
+  <si>
+    <t>₹ 20,232</t>
+  </si>
+  <si>
+    <t>₹ 20,000</t>
+  </si>
+  <si>
+    <t>₹ 16,116</t>
+  </si>
+  <si>
+    <t>₹ 15,000</t>
+  </si>
+  <si>
+    <t>₹ 11,493</t>
+  </si>
+  <si>
+    <t>₹ 10,116</t>
+  </si>
+  <si>
+    <t>₹ 10,016</t>
+  </si>
+  <si>
+    <t>₹ 10,001</t>
+  </si>
+  <si>
+    <t>₹ 10,000</t>
+  </si>
+  <si>
+    <t>₹ 7,722</t>
+  </si>
+  <si>
+    <t>₹ 7,000</t>
+  </si>
+  <si>
+    <t>₹ 6,000</t>
+  </si>
+  <si>
+    <t>₹ 5,116</t>
+  </si>
+  <si>
+    <t>₹ 5,100</t>
+  </si>
+  <si>
+    <t>₹ 5,004</t>
+  </si>
+  <si>
+    <t>₹ 5,001</t>
+  </si>
+  <si>
+    <t>₹ 5,000</t>
+  </si>
+  <si>
+    <t>₹ 3,001</t>
+  </si>
+  <si>
+    <t>₹ 3,000</t>
+  </si>
+  <si>
+    <t>₹ 2,500</t>
+  </si>
+  <si>
+    <t>₹ 2,016</t>
+  </si>
+  <si>
+    <t>₹ 2,000</t>
+  </si>
+  <si>
+    <t>₹ 1,120</t>
+  </si>
+  <si>
+    <t>₹ 1,116</t>
+  </si>
+  <si>
+    <t>₹ 1,016</t>
+  </si>
+  <si>
+    <t>₹ 1,011</t>
+  </si>
+  <si>
+    <t>₹ 1,001</t>
+  </si>
+  <si>
+    <t>₹ 1,000</t>
+  </si>
+  <si>
+    <t>₹ 520</t>
+  </si>
+  <si>
+    <t>₹ 501</t>
+  </si>
+  <si>
+    <t>₹ 120</t>
   </si>
 </sst>
 </file>
@@ -1571,7 +1688,7 @@
   <dimension ref="A1:H203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D205" sqref="D205"/>
+      <selection activeCell="F4" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1627,8 +1744,8 @@
       <c r="E2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="32">
-        <v>350000</v>
+      <c r="F2" s="32" t="s">
+        <v>338</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="23"/>
@@ -1638,19 +1755,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>132</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>340</v>
-      </c>
       <c r="F3" s="32" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="23"/>
@@ -1672,7 +1789,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="24"/>
@@ -1693,8 +1810,8 @@
       <c r="E5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32">
-        <v>150000</v>
+      <c r="F5" s="32" t="s">
+        <v>341</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="24"/>
@@ -1715,8 +1832,8 @@
       <c r="E6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="32">
-        <v>100116</v>
+      <c r="F6" s="32" t="s">
+        <v>342</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="24"/>
@@ -1738,7 +1855,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="24"/>
@@ -1760,7 +1877,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="24"/>
@@ -1782,7 +1899,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="24"/>
@@ -1801,8 +1918,8 @@
       <c r="E10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="32">
-        <v>100000</v>
+      <c r="F10" s="32" t="s">
+        <v>343</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="24"/>
@@ -1823,8 +1940,8 @@
       <c r="E11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="32">
-        <v>100000</v>
+      <c r="F11" s="32" t="s">
+        <v>343</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="24"/>
@@ -1845,8 +1962,8 @@
       <c r="E12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="32">
-        <v>100000</v>
+      <c r="F12" s="32" t="s">
+        <v>343</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="24"/>
@@ -1867,8 +1984,8 @@
       <c r="E13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="32">
-        <v>100000</v>
+      <c r="F13" s="32" t="s">
+        <v>343</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="24"/>
@@ -1889,8 +2006,8 @@
       <c r="E14" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="F14" s="32">
-        <v>100000</v>
+      <c r="F14" s="32" t="s">
+        <v>343</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="24"/>
@@ -1911,8 +2028,8 @@
       <c r="E15" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="32">
-        <v>60000</v>
+      <c r="F15" s="32" t="s">
+        <v>344</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>330</v>
@@ -1937,8 +2054,8 @@
       <c r="E16" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="32">
-        <v>50116</v>
+      <c r="F16" s="32" t="s">
+        <v>345</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="24"/>
@@ -1959,8 +2076,8 @@
       <c r="E17" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="32">
-        <v>50116</v>
+      <c r="F17" s="32" t="s">
+        <v>345</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="24"/>
@@ -1981,8 +2098,8 @@
       <c r="E18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="32">
-        <v>50011</v>
+      <c r="F18" s="32" t="s">
+        <v>346</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>330</v>
@@ -2007,8 +2124,8 @@
       <c r="E19" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="32">
-        <v>50000</v>
+      <c r="F19" s="32" t="s">
+        <v>347</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="24"/>
@@ -2029,8 +2146,8 @@
       <c r="E20" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="32">
-        <v>50000</v>
+      <c r="F20" s="32" t="s">
+        <v>347</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="24"/>
@@ -2051,8 +2168,8 @@
       <c r="E21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="32">
-        <v>50000</v>
+      <c r="F21" s="32" t="s">
+        <v>347</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="24"/>
@@ -2073,8 +2190,8 @@
       <c r="E22" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="32">
-        <v>50000</v>
+      <c r="F22" s="32" t="s">
+        <v>347</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="24"/>
@@ -2095,8 +2212,8 @@
       <c r="E23" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="32">
-        <v>50000</v>
+      <c r="F23" s="32" t="s">
+        <v>347</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="24"/>
@@ -2117,8 +2234,8 @@
       <c r="E24" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="32">
-        <v>50000</v>
+      <c r="F24" s="32" t="s">
+        <v>347</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="24"/>
@@ -2139,8 +2256,8 @@
       <c r="E25" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="F25" s="32">
-        <v>50000</v>
+      <c r="F25" s="32" t="s">
+        <v>347</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="24"/>
@@ -2161,8 +2278,8 @@
       <c r="E26" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="F26" s="32">
-        <v>50000</v>
+      <c r="F26" s="32" t="s">
+        <v>347</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="24"/>
@@ -2183,8 +2300,8 @@
       <c r="E27" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="32">
-        <v>50000</v>
+      <c r="F27" s="32" t="s">
+        <v>347</v>
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="24"/>
@@ -2205,8 +2322,8 @@
       <c r="E28" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="32">
-        <v>50000</v>
+      <c r="F28" s="32" t="s">
+        <v>347</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="24"/>
@@ -2227,8 +2344,8 @@
       <c r="E29" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F29" s="32">
-        <v>50000</v>
+      <c r="F29" s="32" t="s">
+        <v>347</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="24"/>
@@ -2249,8 +2366,8 @@
       <c r="E30" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="32">
-        <v>32500</v>
+      <c r="F30" s="32" t="s">
+        <v>348</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>330</v>
@@ -2275,8 +2392,8 @@
       <c r="E31" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32">
-        <v>25000</v>
+      <c r="F31" s="32" t="s">
+        <v>349</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="24"/>
@@ -2297,8 +2414,8 @@
       <c r="E32" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F32" s="32">
-        <v>25000</v>
+      <c r="F32" s="32" t="s">
+        <v>349</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="24"/>
@@ -2319,8 +2436,8 @@
       <c r="E33" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="32">
-        <v>25000</v>
+      <c r="F33" s="32" t="s">
+        <v>349</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="24"/>
@@ -2341,8 +2458,8 @@
       <c r="E34" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="32">
-        <v>25000</v>
+      <c r="F34" s="32" t="s">
+        <v>349</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="24"/>
@@ -2363,8 +2480,8 @@
       <c r="E35" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="32">
-        <v>25000</v>
+      <c r="F35" s="32" t="s">
+        <v>349</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="24"/>
@@ -2385,8 +2502,8 @@
       <c r="E36" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F36" s="32">
-        <v>25000</v>
+      <c r="F36" s="32" t="s">
+        <v>349</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="24"/>
@@ -2407,8 +2524,8 @@
       <c r="E37" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="F37" s="32">
-        <v>25000</v>
+      <c r="F37" s="32" t="s">
+        <v>349</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="24"/>
@@ -2429,8 +2546,8 @@
       <c r="E38" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F38" s="32">
-        <v>20232</v>
+      <c r="F38" s="32" t="s">
+        <v>350</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="24"/>
@@ -2451,8 +2568,8 @@
       <c r="E39" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F39" s="32">
-        <v>20000</v>
+      <c r="F39" s="32" t="s">
+        <v>351</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="24"/>
@@ -2471,8 +2588,8 @@
       <c r="E40" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F40" s="32">
-        <v>20000</v>
+      <c r="F40" s="32" t="s">
+        <v>351</v>
       </c>
       <c r="G40" s="7"/>
       <c r="H40" s="24"/>
@@ -2493,8 +2610,8 @@
       <c r="E41" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="F41" s="32">
-        <v>20000</v>
+      <c r="F41" s="32" t="s">
+        <v>351</v>
       </c>
       <c r="G41" s="7"/>
       <c r="H41" s="24"/>
@@ -2515,8 +2632,8 @@
       <c r="E42" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F42" s="32">
-        <v>20000</v>
+      <c r="F42" s="32" t="s">
+        <v>351</v>
       </c>
       <c r="G42" s="7"/>
       <c r="H42" s="24"/>
@@ -2537,8 +2654,8 @@
       <c r="E43" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F43" s="32">
-        <v>20000</v>
+      <c r="F43" s="32" t="s">
+        <v>351</v>
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="24"/>
@@ -2559,8 +2676,8 @@
       <c r="E44" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F44" s="32">
-        <v>20000</v>
+      <c r="F44" s="32" t="s">
+        <v>351</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>330</v>
@@ -2585,8 +2702,8 @@
       <c r="E45" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F45" s="32">
-        <v>20000</v>
+      <c r="F45" s="32" t="s">
+        <v>351</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>330</v>
@@ -2612,7 +2729,7 @@
         <v>4</v>
       </c>
       <c r="F46" s="32" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="G46" s="7"/>
       <c r="H46" s="24"/>
@@ -2634,7 +2751,7 @@
         <v>42</v>
       </c>
       <c r="F47" s="32" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="24"/>
@@ -2655,8 +2772,8 @@
       <c r="E48" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="32">
-        <v>16116</v>
+      <c r="F48" s="32" t="s">
+        <v>352</v>
       </c>
       <c r="G48" s="7"/>
       <c r="H48" s="24"/>
@@ -2677,8 +2794,8 @@
       <c r="E49" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="F49" s="32">
-        <v>15000</v>
+      <c r="F49" s="32" t="s">
+        <v>353</v>
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="24"/>
@@ -2699,8 +2816,8 @@
       <c r="E50" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="32">
-        <v>11493</v>
+      <c r="F50" s="32" t="s">
+        <v>354</v>
       </c>
       <c r="G50" s="7"/>
       <c r="H50" s="24"/>
@@ -2721,8 +2838,8 @@
       <c r="E51" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F51" s="32">
-        <v>10116</v>
+      <c r="F51" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="24"/>
@@ -2743,8 +2860,8 @@
       <c r="E52" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F52" s="32">
-        <v>10116</v>
+      <c r="F52" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G52" s="7"/>
       <c r="H52" s="24"/>
@@ -2765,8 +2882,8 @@
       <c r="E53" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F53" s="32">
-        <v>10116</v>
+      <c r="F53" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G53" s="7"/>
       <c r="H53" s="24"/>
@@ -2787,8 +2904,8 @@
       <c r="E54" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F54" s="32">
-        <v>10116</v>
+      <c r="F54" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G54" s="7"/>
       <c r="H54" s="24"/>
@@ -2809,8 +2926,8 @@
       <c r="E55" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F55" s="32">
-        <v>10116</v>
+      <c r="F55" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G55" s="7"/>
       <c r="H55" s="24"/>
@@ -2831,8 +2948,8 @@
       <c r="E56" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="32">
-        <v>10116</v>
+      <c r="F56" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G56" s="7"/>
       <c r="H56" s="24"/>
@@ -2851,8 +2968,8 @@
       <c r="E57" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F57" s="32">
-        <v>10116</v>
+      <c r="F57" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G57" s="7"/>
       <c r="H57" s="24"/>
@@ -2873,8 +2990,8 @@
       <c r="E58" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F58" s="32">
-        <v>10116</v>
+      <c r="F58" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G58" s="7"/>
       <c r="H58" s="24"/>
@@ -2895,8 +3012,8 @@
       <c r="E59" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F59" s="32">
-        <v>10116</v>
+      <c r="F59" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G59" s="7"/>
       <c r="H59" s="24"/>
@@ -2917,8 +3034,8 @@
       <c r="E60" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F60" s="32">
-        <v>10116</v>
+      <c r="F60" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G60" s="7"/>
       <c r="H60" s="24"/>
@@ -2939,8 +3056,8 @@
       <c r="E61" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F61" s="32">
-        <v>10116</v>
+      <c r="F61" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G61" s="31"/>
       <c r="H61" s="25"/>
@@ -2961,8 +3078,8 @@
       <c r="E62" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F62" s="32">
-        <v>10116</v>
+      <c r="F62" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G62" s="7"/>
       <c r="H62" s="24"/>
@@ -2983,8 +3100,8 @@
       <c r="E63" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F63" s="32">
-        <v>10116</v>
+      <c r="F63" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G63" s="7"/>
       <c r="H63" s="24"/>
@@ -3005,8 +3122,8 @@
       <c r="E64" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F64" s="32">
-        <v>10116</v>
+      <c r="F64" s="32" t="s">
+        <v>355</v>
       </c>
       <c r="G64" s="7"/>
       <c r="H64" s="24"/>
@@ -3027,8 +3144,8 @@
       <c r="E65" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F65" s="32">
-        <v>10016</v>
+      <c r="F65" s="32" t="s">
+        <v>356</v>
       </c>
       <c r="G65" s="7"/>
       <c r="H65" s="24"/>
@@ -3049,8 +3166,8 @@
       <c r="E66" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F66" s="32">
-        <v>10001</v>
+      <c r="F66" s="32" t="s">
+        <v>357</v>
       </c>
       <c r="G66" s="11"/>
       <c r="H66" s="23"/>
@@ -3071,8 +3188,8 @@
       <c r="E67" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F67" s="32">
-        <v>10001</v>
+      <c r="F67" s="32" t="s">
+        <v>357</v>
       </c>
       <c r="G67" s="7"/>
       <c r="H67" s="24"/>
@@ -3093,8 +3210,8 @@
       <c r="E68" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F68" s="32">
-        <v>10001</v>
+      <c r="F68" s="32" t="s">
+        <v>357</v>
       </c>
       <c r="G68" s="7"/>
       <c r="H68" s="24"/>
@@ -3113,8 +3230,8 @@
       <c r="E69" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F69" s="32">
-        <v>10001</v>
+      <c r="F69" s="32" t="s">
+        <v>357</v>
       </c>
       <c r="G69" s="7"/>
       <c r="H69" s="24"/>
@@ -3135,8 +3252,8 @@
       <c r="E70" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F70" s="32">
-        <v>10000</v>
+      <c r="F70" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G70" s="7"/>
       <c r="H70" s="24"/>
@@ -3157,8 +3274,8 @@
       <c r="E71" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F71" s="32">
-        <v>10000</v>
+      <c r="F71" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G71" s="7"/>
       <c r="H71" s="24"/>
@@ -3179,8 +3296,8 @@
       <c r="E72" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F72" s="32">
-        <v>10000</v>
+      <c r="F72" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G72" s="7"/>
       <c r="H72" s="24"/>
@@ -3201,8 +3318,8 @@
       <c r="E73" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F73" s="32">
-        <v>10000</v>
+      <c r="F73" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G73" s="7"/>
       <c r="H73" s="24"/>
@@ -3223,8 +3340,8 @@
       <c r="E74" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F74" s="32">
-        <v>10000</v>
+      <c r="F74" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G74" s="7"/>
       <c r="H74" s="24"/>
@@ -3245,8 +3362,8 @@
       <c r="E75" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F75" s="32">
-        <v>10000</v>
+      <c r="F75" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G75" s="7"/>
       <c r="H75" s="24"/>
@@ -3267,8 +3384,8 @@
       <c r="E76" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F76" s="32">
-        <v>10000</v>
+      <c r="F76" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G76" s="7"/>
       <c r="H76" s="24"/>
@@ -3289,8 +3406,8 @@
       <c r="E77" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F77" s="32">
-        <v>10000</v>
+      <c r="F77" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G77" s="7"/>
       <c r="H77" s="24"/>
@@ -3311,8 +3428,8 @@
       <c r="E78" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F78" s="32">
-        <v>10000</v>
+      <c r="F78" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G78" s="7"/>
       <c r="H78" s="24"/>
@@ -3333,8 +3450,8 @@
       <c r="E79" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F79" s="32">
-        <v>10000</v>
+      <c r="F79" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G79" s="7"/>
       <c r="H79" s="24"/>
@@ -3355,8 +3472,8 @@
       <c r="E80" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F80" s="32">
-        <v>10000</v>
+      <c r="F80" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G80" s="7"/>
       <c r="H80" s="24"/>
@@ -3377,8 +3494,8 @@
       <c r="E81" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F81" s="32">
-        <v>10000</v>
+      <c r="F81" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G81" s="7"/>
       <c r="H81" s="24"/>
@@ -3399,8 +3516,8 @@
       <c r="E82" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F82" s="32">
-        <v>10000</v>
+      <c r="F82" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G82" s="7"/>
       <c r="H82" s="24"/>
@@ -3421,8 +3538,8 @@
       <c r="E83" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F83" s="32">
-        <v>10000</v>
+      <c r="F83" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G83" s="7"/>
       <c r="H83" s="24"/>
@@ -3443,8 +3560,8 @@
       <c r="E84" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F84" s="32">
-        <v>10000</v>
+      <c r="F84" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G84" s="7"/>
       <c r="H84" s="24"/>
@@ -3465,8 +3582,8 @@
       <c r="E85" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F85" s="32">
-        <v>10000</v>
+      <c r="F85" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G85" s="7"/>
       <c r="H85" s="24"/>
@@ -3487,8 +3604,8 @@
       <c r="E86" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F86" s="32">
-        <v>10000</v>
+      <c r="F86" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G86" s="7"/>
       <c r="H86" s="24"/>
@@ -3509,8 +3626,8 @@
       <c r="E87" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="F87" s="32">
-        <v>10000</v>
+      <c r="F87" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G87" s="7"/>
       <c r="H87" s="24"/>
@@ -3531,8 +3648,8 @@
       <c r="E88" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F88" s="32">
-        <v>10000</v>
+      <c r="F88" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G88" s="7"/>
       <c r="H88" s="24"/>
@@ -3553,8 +3670,8 @@
       <c r="E89" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F89" s="32">
-        <v>10000</v>
+      <c r="F89" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G89" s="7"/>
       <c r="H89" s="24"/>
@@ -3575,8 +3692,8 @@
       <c r="E90" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F90" s="32">
-        <v>10000</v>
+      <c r="F90" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G90" s="7"/>
       <c r="H90" s="24"/>
@@ -3597,8 +3714,8 @@
       <c r="E91" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F91" s="32">
-        <v>10000</v>
+      <c r="F91" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G91" s="7"/>
       <c r="H91" s="24"/>
@@ -3619,8 +3736,8 @@
       <c r="E92" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F92" s="32">
-        <v>10000</v>
+      <c r="F92" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G92" s="7"/>
       <c r="H92" s="24"/>
@@ -3641,8 +3758,8 @@
       <c r="E93" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F93" s="32">
-        <v>10000</v>
+      <c r="F93" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G93" s="7"/>
       <c r="H93" s="24"/>
@@ -3663,8 +3780,8 @@
       <c r="E94" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F94" s="32">
-        <v>10000</v>
+      <c r="F94" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G94" s="7"/>
       <c r="H94" s="24"/>
@@ -3685,8 +3802,8 @@
       <c r="E95" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F95" s="32">
-        <v>10000</v>
+      <c r="F95" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G95" s="7"/>
       <c r="H95" s="24"/>
@@ -3707,8 +3824,8 @@
       <c r="E96" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F96" s="32">
-        <v>10000</v>
+      <c r="F96" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G96" s="7"/>
       <c r="H96" s="24"/>
@@ -3729,8 +3846,8 @@
       <c r="E97" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F97" s="32">
-        <v>10000</v>
+      <c r="F97" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G97" s="7"/>
       <c r="H97" s="24"/>
@@ -3751,8 +3868,8 @@
       <c r="E98" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F98" s="32">
-        <v>10000</v>
+      <c r="F98" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G98" s="7"/>
       <c r="H98" s="24"/>
@@ -3773,8 +3890,8 @@
       <c r="E99" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F99" s="32">
-        <v>10000</v>
+      <c r="F99" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G99" s="7"/>
       <c r="H99" s="24"/>
@@ -3795,8 +3912,8 @@
       <c r="E100" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F100" s="32">
-        <v>10000</v>
+      <c r="F100" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G100" s="7"/>
       <c r="H100" s="24"/>
@@ -3817,8 +3934,8 @@
       <c r="E101" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F101" s="32">
-        <v>10000</v>
+      <c r="F101" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G101" s="7"/>
       <c r="H101" s="24"/>
@@ -3839,8 +3956,8 @@
       <c r="E102" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F102" s="32">
-        <v>10000</v>
+      <c r="F102" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G102" s="12"/>
       <c r="H102" s="26"/>
@@ -3861,8 +3978,8 @@
       <c r="E103" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F103" s="32">
-        <v>10000</v>
+      <c r="F103" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G103" s="12"/>
       <c r="H103" s="26"/>
@@ -3883,8 +4000,8 @@
       <c r="E104" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F104" s="32">
-        <v>10000</v>
+      <c r="F104" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G104" s="12"/>
       <c r="H104" s="26"/>
@@ -3905,8 +4022,8 @@
       <c r="E105" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F105" s="32">
-        <v>10000</v>
+      <c r="F105" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G105" s="7"/>
       <c r="H105" s="24"/>
@@ -3927,8 +4044,8 @@
       <c r="E106" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F106" s="32">
-        <v>10000</v>
+      <c r="F106" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G106" s="7"/>
       <c r="H106" s="24"/>
@@ -3949,8 +4066,8 @@
       <c r="E107" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F107" s="32">
-        <v>10000</v>
+      <c r="F107" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G107" s="7"/>
       <c r="H107" s="24"/>
@@ -3971,8 +4088,8 @@
       <c r="E108" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="F108" s="32">
-        <v>10000</v>
+      <c r="F108" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G108" s="7"/>
       <c r="H108" s="24"/>
@@ -3993,8 +4110,8 @@
       <c r="E109" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="F109" s="32">
-        <v>10000</v>
+      <c r="F109" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G109" s="7"/>
       <c r="H109" s="24"/>
@@ -4011,8 +4128,8 @@
         <v>302</v>
       </c>
       <c r="E110" s="12"/>
-      <c r="F110" s="32">
-        <v>10000</v>
+      <c r="F110" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G110" s="7"/>
       <c r="H110" s="24"/>
@@ -4033,8 +4150,8 @@
       <c r="E111" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F111" s="32">
-        <v>10000</v>
+      <c r="F111" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G111" s="7"/>
       <c r="H111" s="24"/>
@@ -4055,8 +4172,8 @@
       <c r="E112" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="F112" s="32">
-        <v>10000</v>
+      <c r="F112" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G112" s="7"/>
       <c r="H112" s="24"/>
@@ -4077,8 +4194,8 @@
       <c r="E113" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F113" s="32">
-        <v>10000</v>
+      <c r="F113" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G113" s="7"/>
       <c r="H113" s="24"/>
@@ -4099,8 +4216,8 @@
       <c r="E114" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F114" s="32">
-        <v>10000</v>
+      <c r="F114" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G114" s="7"/>
       <c r="H114" s="24"/>
@@ -4121,8 +4238,8 @@
       <c r="E115" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F115" s="32">
-        <v>10000</v>
+      <c r="F115" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="G115" s="7"/>
       <c r="H115" s="24"/>
@@ -4143,8 +4260,8 @@
       <c r="E116" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F116" s="32">
-        <v>7722</v>
+      <c r="F116" s="32" t="s">
+        <v>359</v>
       </c>
       <c r="G116" s="7"/>
       <c r="H116" s="24"/>
@@ -4165,8 +4282,8 @@
       <c r="E117" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F117" s="32">
-        <v>7000</v>
+      <c r="F117" s="32" t="s">
+        <v>360</v>
       </c>
       <c r="G117" s="7"/>
       <c r="H117" s="24"/>
@@ -4187,8 +4304,8 @@
       <c r="E118" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F118" s="32">
-        <v>7000</v>
+      <c r="F118" s="32" t="s">
+        <v>360</v>
       </c>
       <c r="G118" s="7"/>
       <c r="H118" s="24"/>
@@ -4207,8 +4324,8 @@
         <v>314</v>
       </c>
       <c r="E119" s="13"/>
-      <c r="F119" s="32">
-        <v>6000</v>
+      <c r="F119" s="32" t="s">
+        <v>361</v>
       </c>
       <c r="G119" s="7"/>
       <c r="H119" s="24"/>
@@ -4229,8 +4346,8 @@
       <c r="E120" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F120" s="32">
-        <v>5116</v>
+      <c r="F120" s="32" t="s">
+        <v>362</v>
       </c>
       <c r="G120" s="7"/>
       <c r="H120" s="24"/>
@@ -4251,8 +4368,8 @@
       <c r="E121" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F121" s="32">
-        <v>5116</v>
+      <c r="F121" s="32" t="s">
+        <v>362</v>
       </c>
       <c r="G121" s="7"/>
       <c r="H121" s="24"/>
@@ -4271,8 +4388,8 @@
       <c r="E122" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F122" s="32">
-        <v>5116</v>
+      <c r="F122" s="32" t="s">
+        <v>362</v>
       </c>
       <c r="G122" s="7"/>
       <c r="H122" s="24"/>
@@ -4293,8 +4410,8 @@
       <c r="E123" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F123" s="32">
-        <v>5116</v>
+      <c r="F123" s="32" t="s">
+        <v>362</v>
       </c>
       <c r="G123" s="7"/>
       <c r="H123" s="24"/>
@@ -4315,8 +4432,8 @@
       <c r="E124" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F124" s="32">
-        <v>5116</v>
+      <c r="F124" s="32" t="s">
+        <v>362</v>
       </c>
       <c r="G124" s="7"/>
       <c r="H124" s="24"/>
@@ -4337,8 +4454,8 @@
       <c r="E125" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F125" s="32">
-        <v>5116</v>
+      <c r="F125" s="32" t="s">
+        <v>362</v>
       </c>
       <c r="G125" s="7"/>
       <c r="H125" s="24"/>
@@ -4359,8 +4476,8 @@
       <c r="E126" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F126" s="32">
-        <v>5116</v>
+      <c r="F126" s="32" t="s">
+        <v>362</v>
       </c>
       <c r="G126" s="7"/>
       <c r="H126" s="24"/>
@@ -4379,8 +4496,8 @@
       <c r="E127" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F127" s="32">
-        <v>5116</v>
+      <c r="F127" s="32" t="s">
+        <v>362</v>
       </c>
       <c r="G127" s="7"/>
       <c r="H127" s="24"/>
@@ -4399,8 +4516,8 @@
       <c r="E128" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F128" s="32">
-        <v>5116</v>
+      <c r="F128" s="32" t="s">
+        <v>362</v>
       </c>
       <c r="G128" s="7"/>
       <c r="H128" s="24"/>
@@ -4421,8 +4538,8 @@
       <c r="E129" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F129" s="32">
-        <v>5100</v>
+      <c r="F129" s="32" t="s">
+        <v>363</v>
       </c>
       <c r="G129" s="7"/>
       <c r="H129" s="24"/>
@@ -4443,8 +4560,8 @@
       <c r="E130" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F130" s="32">
-        <v>5004</v>
+      <c r="F130" s="32" t="s">
+        <v>364</v>
       </c>
       <c r="G130" s="7"/>
       <c r="H130" s="24"/>
@@ -4465,8 +4582,8 @@
       <c r="E131" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F131" s="32">
-        <v>5004</v>
+      <c r="F131" s="32" t="s">
+        <v>364</v>
       </c>
       <c r="G131" s="7"/>
       <c r="H131" s="24"/>
@@ -4485,8 +4602,8 @@
       <c r="E132" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F132" s="32">
-        <v>5001</v>
+      <c r="F132" s="32" t="s">
+        <v>365</v>
       </c>
       <c r="G132" s="7"/>
       <c r="H132" s="24"/>
@@ -4505,8 +4622,8 @@
       <c r="E133" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F133" s="32">
-        <v>5001</v>
+      <c r="F133" s="32" t="s">
+        <v>365</v>
       </c>
       <c r="G133" s="7"/>
       <c r="H133" s="24"/>
@@ -4527,8 +4644,8 @@
       <c r="E134" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F134" s="32">
-        <v>5001</v>
+      <c r="F134" s="32" t="s">
+        <v>365</v>
       </c>
       <c r="G134" s="7"/>
       <c r="H134" s="24"/>
@@ -4545,8 +4662,8 @@
         <v>227</v>
       </c>
       <c r="E135" s="13"/>
-      <c r="F135" s="32">
-        <v>5001</v>
+      <c r="F135" s="32" t="s">
+        <v>365</v>
       </c>
       <c r="G135" s="7"/>
       <c r="H135" s="24"/>
@@ -4567,8 +4684,8 @@
       <c r="E136" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F136" s="32">
-        <v>5000</v>
+      <c r="F136" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G136" s="7"/>
       <c r="H136" s="24"/>
@@ -4589,8 +4706,8 @@
       <c r="E137" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F137" s="32">
-        <v>5000</v>
+      <c r="F137" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G137" s="11"/>
       <c r="H137" s="23"/>
@@ -4611,8 +4728,8 @@
       <c r="E138" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F138" s="32">
-        <v>5000</v>
+      <c r="F138" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G138" s="7"/>
       <c r="H138" s="24"/>
@@ -4633,8 +4750,8 @@
       <c r="E139" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F139" s="32">
-        <v>5000</v>
+      <c r="F139" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G139" s="7"/>
       <c r="H139" s="24"/>
@@ -4655,8 +4772,8 @@
       <c r="E140" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F140" s="32">
-        <v>5000</v>
+      <c r="F140" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G140" s="7"/>
       <c r="H140" s="24"/>
@@ -4677,8 +4794,8 @@
       <c r="E141" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F141" s="32">
-        <v>5000</v>
+      <c r="F141" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G141" s="7"/>
       <c r="H141" s="24"/>
@@ -4699,8 +4816,8 @@
       <c r="E142" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F142" s="32">
-        <v>5000</v>
+      <c r="F142" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G142" s="7"/>
       <c r="H142" s="24"/>
@@ -4719,8 +4836,8 @@
       <c r="E143" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F143" s="32">
-        <v>5000</v>
+      <c r="F143" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G143" s="7"/>
       <c r="H143" s="24"/>
@@ -4741,8 +4858,8 @@
       <c r="E144" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F144" s="32">
-        <v>5000</v>
+      <c r="F144" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G144" s="7"/>
       <c r="H144" s="24"/>
@@ -4763,8 +4880,8 @@
       <c r="E145" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F145" s="32">
-        <v>5000</v>
+      <c r="F145" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G145" s="7"/>
       <c r="H145" s="24"/>
@@ -4783,8 +4900,8 @@
       <c r="E146" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F146" s="33">
-        <v>5000</v>
+      <c r="F146" s="33" t="s">
+        <v>366</v>
       </c>
       <c r="G146" s="7"/>
       <c r="H146" s="24"/>
@@ -4805,8 +4922,8 @@
       <c r="E147" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F147" s="32">
-        <v>5000</v>
+      <c r="F147" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G147" s="7"/>
       <c r="H147" s="24"/>
@@ -4827,8 +4944,8 @@
       <c r="E148" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F148" s="32">
-        <v>5000</v>
+      <c r="F148" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G148" s="7"/>
       <c r="H148" s="24"/>
@@ -4849,8 +4966,8 @@
       <c r="E149" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F149" s="32">
-        <v>5000</v>
+      <c r="F149" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G149" s="7"/>
       <c r="H149" s="24"/>
@@ -4869,8 +4986,8 @@
       <c r="E150" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F150" s="32">
-        <v>5000</v>
+      <c r="F150" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G150" s="7"/>
       <c r="H150" s="24"/>
@@ -4889,8 +5006,8 @@
       <c r="E151" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F151" s="32">
-        <v>5000</v>
+      <c r="F151" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G151" s="7"/>
       <c r="H151" s="24"/>
@@ -4909,8 +5026,8 @@
       <c r="E152" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F152" s="32">
-        <v>5000</v>
+      <c r="F152" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G152" s="7"/>
       <c r="H152" s="24"/>
@@ -4931,8 +5048,8 @@
       <c r="E153" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F153" s="32">
-        <v>5000</v>
+      <c r="F153" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G153" s="7"/>
       <c r="H153" s="24"/>
@@ -4953,8 +5070,8 @@
       <c r="E154" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F154" s="32">
-        <v>5000</v>
+      <c r="F154" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G154" s="7"/>
       <c r="H154" s="24"/>
@@ -4975,8 +5092,8 @@
       <c r="E155" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F155" s="32">
-        <v>5000</v>
+      <c r="F155" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G155" s="7"/>
       <c r="H155" s="24"/>
@@ -4995,8 +5112,8 @@
       <c r="E156" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F156" s="32">
-        <v>5000</v>
+      <c r="F156" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G156" s="7"/>
       <c r="H156" s="24"/>
@@ -5017,8 +5134,8 @@
       <c r="E157" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F157" s="32">
-        <v>5000</v>
+      <c r="F157" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G157" s="7"/>
       <c r="H157" s="24"/>
@@ -5039,8 +5156,8 @@
       <c r="E158" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F158" s="32">
-        <v>5000</v>
+      <c r="F158" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G158" s="7"/>
       <c r="H158" s="24"/>
@@ -5061,8 +5178,8 @@
       <c r="E159" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F159" s="32">
-        <v>5000</v>
+      <c r="F159" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G159" s="7"/>
       <c r="H159" s="24"/>
@@ -5083,8 +5200,8 @@
       <c r="E160" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F160" s="32">
-        <v>5000</v>
+      <c r="F160" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G160" s="7"/>
       <c r="H160" s="24"/>
@@ -5105,8 +5222,8 @@
       <c r="E161" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F161" s="32">
-        <v>5000</v>
+      <c r="F161" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G161" s="7"/>
       <c r="H161" s="24"/>
@@ -5123,8 +5240,8 @@
         <v>162</v>
       </c>
       <c r="E162" s="13"/>
-      <c r="F162" s="32">
-        <v>5000</v>
+      <c r="F162" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G162" s="7"/>
       <c r="H162" s="24"/>
@@ -5145,8 +5262,8 @@
       <c r="E163" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="F163" s="32">
-        <v>5000</v>
+      <c r="F163" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G163" s="7"/>
       <c r="H163" s="24"/>
@@ -5167,8 +5284,8 @@
       <c r="E164" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F164" s="32">
-        <v>5000</v>
+      <c r="F164" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G164" s="7"/>
       <c r="H164" s="24"/>
@@ -5189,8 +5306,8 @@
       <c r="E165" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F165" s="32">
-        <v>5000</v>
+      <c r="F165" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G165" s="7"/>
       <c r="H165" s="24"/>
@@ -5211,8 +5328,8 @@
       <c r="E166" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F166" s="32">
-        <v>5000</v>
+      <c r="F166" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G166" s="7"/>
       <c r="H166" s="24"/>
@@ -5231,8 +5348,8 @@
         <v>301</v>
       </c>
       <c r="E167" s="7"/>
-      <c r="F167" s="32">
-        <v>5000</v>
+      <c r="F167" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G167" s="7"/>
       <c r="H167" s="24"/>
@@ -5253,8 +5370,8 @@
       <c r="E168" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="F168" s="32">
-        <v>5000</v>
+      <c r="F168" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G168" s="7"/>
       <c r="H168" s="24"/>
@@ -5275,8 +5392,8 @@
       <c r="E169" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="F169" s="32">
-        <v>5000</v>
+      <c r="F169" s="32" t="s">
+        <v>366</v>
       </c>
       <c r="G169" s="7"/>
       <c r="H169" s="24"/>
@@ -5297,8 +5414,8 @@
       <c r="E170" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="F170" s="32">
-        <v>3001</v>
+      <c r="F170" s="32" t="s">
+        <v>367</v>
       </c>
       <c r="G170" s="7"/>
       <c r="H170" s="24"/>
@@ -5317,8 +5434,8 @@
       <c r="E171" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F171" s="32">
-        <v>3000</v>
+      <c r="F171" s="32" t="s">
+        <v>368</v>
       </c>
       <c r="G171" s="7"/>
       <c r="H171" s="24"/>
@@ -5337,8 +5454,8 @@
       <c r="E172" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F172" s="32">
-        <v>3000</v>
+      <c r="F172" s="32" t="s">
+        <v>368</v>
       </c>
       <c r="G172" s="7"/>
       <c r="H172" s="24"/>
@@ -5357,8 +5474,8 @@
       <c r="E173" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F173" s="32">
-        <v>3000</v>
+      <c r="F173" s="32" t="s">
+        <v>368</v>
       </c>
       <c r="G173" s="7"/>
       <c r="H173" s="24"/>
@@ -5379,8 +5496,8 @@
       <c r="E174" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="F174" s="32">
-        <v>3000</v>
+      <c r="F174" s="32" t="s">
+        <v>368</v>
       </c>
       <c r="G174" s="7"/>
       <c r="H174" s="24"/>
@@ -5401,8 +5518,8 @@
       <c r="E175" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F175" s="32">
-        <v>2500</v>
+      <c r="F175" s="32" t="s">
+        <v>369</v>
       </c>
       <c r="G175" s="7"/>
       <c r="H175" s="24"/>
@@ -5423,8 +5540,8 @@
       <c r="E176" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F176" s="32">
-        <v>2016</v>
+      <c r="F176" s="32" t="s">
+        <v>370</v>
       </c>
       <c r="G176" s="7"/>
       <c r="H176" s="24"/>
@@ -5443,8 +5560,8 @@
       <c r="E177" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F177" s="32">
-        <v>2000</v>
+      <c r="F177" s="32" t="s">
+        <v>371</v>
       </c>
       <c r="G177" s="7"/>
       <c r="H177" s="24"/>
@@ -5465,8 +5582,8 @@
       <c r="E178" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F178" s="32">
-        <v>2000</v>
+      <c r="F178" s="32" t="s">
+        <v>371</v>
       </c>
       <c r="G178" s="7"/>
       <c r="H178" s="24"/>
@@ -5487,8 +5604,8 @@
       <c r="E179" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F179" s="32">
-        <v>2000</v>
+      <c r="F179" s="32" t="s">
+        <v>371</v>
       </c>
       <c r="G179" s="7"/>
       <c r="H179" s="24"/>
@@ -5507,8 +5624,8 @@
       <c r="E180" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F180" s="32">
-        <v>2000</v>
+      <c r="F180" s="32" t="s">
+        <v>371</v>
       </c>
       <c r="G180" s="7"/>
       <c r="H180" s="24"/>
@@ -5527,8 +5644,8 @@
       <c r="E181" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F181" s="32">
-        <v>2000</v>
+      <c r="F181" s="32" t="s">
+        <v>371</v>
       </c>
       <c r="G181" s="7"/>
       <c r="H181" s="24"/>
@@ -5549,8 +5666,8 @@
       <c r="E182" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="F182" s="32">
-        <v>2000</v>
+      <c r="F182" s="32" t="s">
+        <v>371</v>
       </c>
       <c r="G182" s="7"/>
       <c r="H182" s="24"/>
@@ -5569,8 +5686,8 @@
       <c r="E183" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F183" s="32">
-        <v>1120</v>
+      <c r="F183" s="32" t="s">
+        <v>372</v>
       </c>
       <c r="G183" s="7"/>
       <c r="H183" s="24"/>
@@ -5591,8 +5708,8 @@
       <c r="E184" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F184" s="32">
-        <v>1116</v>
+      <c r="F184" s="32" t="s">
+        <v>373</v>
       </c>
       <c r="G184" s="7"/>
       <c r="H184" s="24"/>
@@ -5613,8 +5730,8 @@
       <c r="E185" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F185" s="32">
-        <v>1116</v>
+      <c r="F185" s="32" t="s">
+        <v>373</v>
       </c>
       <c r="G185" s="7"/>
       <c r="H185" s="24"/>
@@ -5635,8 +5752,8 @@
       <c r="E186" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F186" s="32">
-        <v>1116</v>
+      <c r="F186" s="32" t="s">
+        <v>373</v>
       </c>
       <c r="G186" s="7"/>
       <c r="H186" s="24"/>
@@ -5657,8 +5774,8 @@
       <c r="E187" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F187" s="32">
-        <v>1116</v>
+      <c r="F187" s="32" t="s">
+        <v>373</v>
       </c>
       <c r="G187" s="7"/>
       <c r="H187" s="24"/>
@@ -5679,8 +5796,8 @@
       <c r="E188" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F188" s="32">
-        <v>1116</v>
+      <c r="F188" s="32" t="s">
+        <v>373</v>
       </c>
       <c r="G188" s="7"/>
       <c r="H188" s="24"/>
@@ -5701,8 +5818,8 @@
       <c r="E189" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F189" s="32">
-        <v>1016</v>
+      <c r="F189" s="32" t="s">
+        <v>374</v>
       </c>
       <c r="G189" s="7"/>
       <c r="H189" s="24"/>
@@ -5723,8 +5840,8 @@
       <c r="E190" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F190" s="32">
-        <v>1011</v>
+      <c r="F190" s="32" t="s">
+        <v>375</v>
       </c>
       <c r="G190" s="7"/>
       <c r="H190" s="24"/>
@@ -5745,8 +5862,8 @@
       <c r="E191" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F191" s="32">
-        <v>1001</v>
+      <c r="F191" s="32" t="s">
+        <v>376</v>
       </c>
       <c r="G191" s="7"/>
       <c r="H191" s="24"/>
@@ -5765,8 +5882,8 @@
       <c r="E192" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F192" s="32">
-        <v>1001</v>
+      <c r="F192" s="32" t="s">
+        <v>376</v>
       </c>
       <c r="G192" s="7"/>
       <c r="H192" s="24"/>
@@ -5785,8 +5902,8 @@
       <c r="E193" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F193" s="32">
-        <v>1001</v>
+      <c r="F193" s="32" t="s">
+        <v>376</v>
       </c>
       <c r="G193" s="7"/>
       <c r="H193" s="24"/>
@@ -5805,8 +5922,8 @@
       <c r="E194" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F194" s="32">
-        <v>1001</v>
+      <c r="F194" s="32" t="s">
+        <v>376</v>
       </c>
       <c r="G194" s="7"/>
       <c r="H194" s="24"/>
@@ -5827,8 +5944,8 @@
       <c r="E195" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F195" s="32">
-        <v>1000</v>
+      <c r="F195" s="32" t="s">
+        <v>377</v>
       </c>
       <c r="G195" s="7"/>
       <c r="H195" s="24"/>
@@ -5847,8 +5964,8 @@
       <c r="E196" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F196" s="32">
-        <v>1000</v>
+      <c r="F196" s="32" t="s">
+        <v>377</v>
       </c>
       <c r="G196" s="7"/>
       <c r="H196" s="24"/>
@@ -5869,8 +5986,8 @@
       <c r="E197" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="F197" s="32">
-        <v>1000</v>
+      <c r="F197" s="32" t="s">
+        <v>377</v>
       </c>
       <c r="G197" s="7"/>
       <c r="H197" s="24"/>
@@ -5889,8 +6006,8 @@
       <c r="E198" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F198" s="32">
-        <v>520</v>
+      <c r="F198" s="32" t="s">
+        <v>378</v>
       </c>
       <c r="G198" s="7"/>
       <c r="H198" s="24"/>
@@ -5909,8 +6026,8 @@
       <c r="E199" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F199" s="32">
-        <v>501</v>
+      <c r="F199" s="32" t="s">
+        <v>379</v>
       </c>
       <c r="G199" s="7"/>
       <c r="H199" s="24"/>
@@ -5929,8 +6046,8 @@
       <c r="E200" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F200" s="32">
-        <v>120</v>
+      <c r="F200" s="32" t="s">
+        <v>380</v>
       </c>
       <c r="G200" s="7"/>
       <c r="H200" s="24"/>

</xml_diff>